<commit_message>
Minor improvements, RSI data update
</commit_message>
<xml_diff>
--- a/data/bi_rsi_raw.xlsx
+++ b/data/bi_rsi_raw.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RetnoAndrini\Departemen Statistik\Survei\SPE\2021\1. Januari\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\retno_a\Downloads\SPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Tabel 1" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="106">
   <si>
     <t>DESKRIPSI</t>
   </si>
@@ -553,7 +553,10 @@
     <t>Makassar</t>
   </si>
   <si>
-    <t>Feb*</t>
+    <t>Mar*</t>
+  </si>
+  <si>
+    <t>Q1*</t>
   </si>
 </sst>
 </file>
@@ -796,7 +799,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="57">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -1416,19 +1419,6 @@
       <left style="thin">
         <color theme="0"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1440,12 +1430,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="16"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1797,7 +1822,10 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1866,7 +1894,7 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1888,6 +1916,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5270,7 +5304,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="DB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DF20" sqref="DF20"/>
+      <selection pane="topRight" activeCell="DH6" sqref="DH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -5278,8 +5312,8 @@
     <col min="1" max="1" width="44.453125" customWidth="1"/>
     <col min="2" max="62" width="9.36328125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="63" max="63" width="9.36328125" customWidth="1" collapsed="1"/>
-    <col min="64" max="111" width="9.36328125" customWidth="1"/>
-    <col min="112" max="121" width="9.36328125" hidden="1" customWidth="1"/>
+    <col min="64" max="112" width="9.36328125" customWidth="1"/>
+    <col min="113" max="121" width="9.36328125" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="43.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5535,155 +5569,155 @@
       <c r="DQ3" s="2"/>
     </row>
     <row r="4" spans="1:122" ht="18" customHeight="1">
-      <c r="A4" s="138" t="s">
+      <c r="A4" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="M4" s="141"/>
-      <c r="N4" s="144">
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="145">
         <v>2013</v>
       </c>
-      <c r="O4" s="141"/>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="141"/>
-      <c r="R4" s="141"/>
-      <c r="S4" s="141"/>
-      <c r="T4" s="141"/>
-      <c r="U4" s="141"/>
-      <c r="V4" s="141"/>
-      <c r="W4" s="141"/>
-      <c r="X4" s="141"/>
-      <c r="Y4" s="141"/>
-      <c r="Z4" s="144">
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
+      <c r="Q4" s="142"/>
+      <c r="R4" s="142"/>
+      <c r="S4" s="142"/>
+      <c r="T4" s="142"/>
+      <c r="U4" s="142"/>
+      <c r="V4" s="142"/>
+      <c r="W4" s="142"/>
+      <c r="X4" s="142"/>
+      <c r="Y4" s="142"/>
+      <c r="Z4" s="145">
         <v>2014</v>
       </c>
-      <c r="AA4" s="141"/>
-      <c r="AB4" s="141"/>
-      <c r="AC4" s="141"/>
-      <c r="AD4" s="141"/>
-      <c r="AE4" s="141"/>
-      <c r="AF4" s="141"/>
-      <c r="AG4" s="141"/>
-      <c r="AH4" s="141"/>
-      <c r="AI4" s="141"/>
-      <c r="AJ4" s="141"/>
-      <c r="AK4" s="141"/>
-      <c r="AL4" s="144">
+      <c r="AA4" s="142"/>
+      <c r="AB4" s="142"/>
+      <c r="AC4" s="142"/>
+      <c r="AD4" s="142"/>
+      <c r="AE4" s="142"/>
+      <c r="AF4" s="142"/>
+      <c r="AG4" s="142"/>
+      <c r="AH4" s="142"/>
+      <c r="AI4" s="142"/>
+      <c r="AJ4" s="142"/>
+      <c r="AK4" s="142"/>
+      <c r="AL4" s="145">
         <v>2015</v>
       </c>
-      <c r="AM4" s="141"/>
-      <c r="AN4" s="141"/>
-      <c r="AO4" s="141"/>
-      <c r="AP4" s="141"/>
-      <c r="AQ4" s="141"/>
-      <c r="AR4" s="141"/>
-      <c r="AS4" s="141"/>
-      <c r="AT4" s="141"/>
-      <c r="AU4" s="141"/>
-      <c r="AV4" s="141"/>
-      <c r="AW4" s="141"/>
-      <c r="AX4" s="144">
+      <c r="AM4" s="142"/>
+      <c r="AN4" s="142"/>
+      <c r="AO4" s="142"/>
+      <c r="AP4" s="142"/>
+      <c r="AQ4" s="142"/>
+      <c r="AR4" s="142"/>
+      <c r="AS4" s="142"/>
+      <c r="AT4" s="142"/>
+      <c r="AU4" s="142"/>
+      <c r="AV4" s="142"/>
+      <c r="AW4" s="142"/>
+      <c r="AX4" s="145">
         <v>2016</v>
       </c>
-      <c r="AY4" s="141"/>
-      <c r="AZ4" s="141"/>
-      <c r="BA4" s="141"/>
-      <c r="BB4" s="141"/>
-      <c r="BC4" s="141"/>
-      <c r="BD4" s="141"/>
-      <c r="BE4" s="141"/>
-      <c r="BF4" s="141"/>
-      <c r="BG4" s="141"/>
-      <c r="BH4" s="141"/>
-      <c r="BI4" s="141"/>
-      <c r="BJ4" s="144">
+      <c r="AY4" s="142"/>
+      <c r="AZ4" s="142"/>
+      <c r="BA4" s="142"/>
+      <c r="BB4" s="142"/>
+      <c r="BC4" s="142"/>
+      <c r="BD4" s="142"/>
+      <c r="BE4" s="142"/>
+      <c r="BF4" s="142"/>
+      <c r="BG4" s="142"/>
+      <c r="BH4" s="142"/>
+      <c r="BI4" s="142"/>
+      <c r="BJ4" s="145">
         <v>2017</v>
       </c>
-      <c r="BK4" s="141"/>
-      <c r="BL4" s="141"/>
-      <c r="BM4" s="141"/>
-      <c r="BN4" s="141"/>
-      <c r="BO4" s="141"/>
-      <c r="BP4" s="141"/>
-      <c r="BQ4" s="141"/>
-      <c r="BR4" s="141"/>
-      <c r="BS4" s="141"/>
-      <c r="BT4" s="141"/>
-      <c r="BU4" s="141"/>
-      <c r="BV4" s="144">
+      <c r="BK4" s="142"/>
+      <c r="BL4" s="142"/>
+      <c r="BM4" s="142"/>
+      <c r="BN4" s="142"/>
+      <c r="BO4" s="142"/>
+      <c r="BP4" s="142"/>
+      <c r="BQ4" s="142"/>
+      <c r="BR4" s="142"/>
+      <c r="BS4" s="142"/>
+      <c r="BT4" s="142"/>
+      <c r="BU4" s="142"/>
+      <c r="BV4" s="145">
         <v>2018</v>
       </c>
-      <c r="BW4" s="141"/>
-      <c r="BX4" s="141"/>
-      <c r="BY4" s="141"/>
-      <c r="BZ4" s="141"/>
-      <c r="CA4" s="141"/>
-      <c r="CB4" s="141"/>
-      <c r="CC4" s="141"/>
-      <c r="CD4" s="145"/>
-      <c r="CE4" s="141"/>
-      <c r="CF4" s="141"/>
-      <c r="CG4" s="141"/>
-      <c r="CH4" s="144">
+      <c r="BW4" s="142"/>
+      <c r="BX4" s="142"/>
+      <c r="BY4" s="142"/>
+      <c r="BZ4" s="142"/>
+      <c r="CA4" s="142"/>
+      <c r="CB4" s="142"/>
+      <c r="CC4" s="142"/>
+      <c r="CD4" s="146"/>
+      <c r="CE4" s="142"/>
+      <c r="CF4" s="142"/>
+      <c r="CG4" s="142"/>
+      <c r="CH4" s="145">
         <v>2019</v>
       </c>
-      <c r="CI4" s="141"/>
-      <c r="CJ4" s="141"/>
-      <c r="CK4" s="141"/>
-      <c r="CL4" s="141"/>
-      <c r="CM4" s="141"/>
-      <c r="CN4" s="141"/>
-      <c r="CO4" s="141"/>
-      <c r="CP4" s="145"/>
-      <c r="CQ4" s="141"/>
-      <c r="CR4" s="141"/>
-      <c r="CS4" s="141"/>
-      <c r="CT4" s="144">
+      <c r="CI4" s="142"/>
+      <c r="CJ4" s="142"/>
+      <c r="CK4" s="142"/>
+      <c r="CL4" s="142"/>
+      <c r="CM4" s="142"/>
+      <c r="CN4" s="142"/>
+      <c r="CO4" s="142"/>
+      <c r="CP4" s="146"/>
+      <c r="CQ4" s="142"/>
+      <c r="CR4" s="142"/>
+      <c r="CS4" s="142"/>
+      <c r="CT4" s="145">
         <v>2020</v>
       </c>
-      <c r="CU4" s="141"/>
-      <c r="CV4" s="141"/>
-      <c r="CW4" s="141"/>
-      <c r="CX4" s="141"/>
-      <c r="CY4" s="141"/>
-      <c r="CZ4" s="141"/>
-      <c r="DA4" s="141"/>
-      <c r="DB4" s="145"/>
-      <c r="DC4" s="141"/>
-      <c r="DD4" s="141"/>
-      <c r="DE4" s="141"/>
-      <c r="DF4" s="144">
+      <c r="CU4" s="142"/>
+      <c r="CV4" s="142"/>
+      <c r="CW4" s="142"/>
+      <c r="CX4" s="142"/>
+      <c r="CY4" s="142"/>
+      <c r="CZ4" s="142"/>
+      <c r="DA4" s="142"/>
+      <c r="DB4" s="146"/>
+      <c r="DC4" s="142"/>
+      <c r="DD4" s="142"/>
+      <c r="DE4" s="142"/>
+      <c r="DF4" s="145">
         <v>2021</v>
       </c>
-      <c r="DG4" s="141"/>
-      <c r="DH4" s="141"/>
-      <c r="DI4" s="141"/>
-      <c r="DJ4" s="141"/>
-      <c r="DK4" s="141"/>
-      <c r="DL4" s="141"/>
-      <c r="DM4" s="141"/>
-      <c r="DN4" s="145"/>
-      <c r="DO4" s="141"/>
-      <c r="DP4" s="141"/>
-      <c r="DQ4" s="141"/>
-      <c r="DR4" s="142" t="s">
+      <c r="DG4" s="142"/>
+      <c r="DH4" s="142"/>
+      <c r="DI4" s="142"/>
+      <c r="DJ4" s="142"/>
+      <c r="DK4" s="142"/>
+      <c r="DL4" s="142"/>
+      <c r="DM4" s="142"/>
+      <c r="DN4" s="146"/>
+      <c r="DO4" s="142"/>
+      <c r="DP4" s="142"/>
+      <c r="DQ4" s="142"/>
+      <c r="DR4" s="143" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:122" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="139"/>
+      <c r="A5" s="140"/>
       <c r="B5" s="71" t="s">
         <v>2</v>
       </c>
@@ -6012,10 +6046,10 @@
         <v>2</v>
       </c>
       <c r="DG5" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="DH5" s="50" t="s">
         <v>104</v>
-      </c>
-      <c r="DH5" s="50" t="s">
-        <v>4</v>
       </c>
       <c r="DI5" s="50" t="s">
         <v>5</v>
@@ -6044,7 +6078,7 @@
       <c r="DQ5" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="DR5" s="143"/>
+      <c r="DR5" s="144"/>
     </row>
     <row r="6" spans="1:122" ht="18" customHeight="1">
       <c r="A6" s="69" t="s">
@@ -6455,9 +6489,11 @@
         <v>119.26411035824223</v>
       </c>
       <c r="DG6" s="54">
-        <v>119.79755716895137</v>
-      </c>
-      <c r="DH6" s="54"/>
+        <v>117.94518358926754</v>
+      </c>
+      <c r="DH6" s="54">
+        <v>117.76645813555905</v>
+      </c>
       <c r="DI6" s="54"/>
       <c r="DJ6" s="54"/>
       <c r="DK6" s="54"/>
@@ -6880,9 +6916,11 @@
         <v>223.9037449199617</v>
       </c>
       <c r="DG7" s="58">
-        <v>222.11368748246608</v>
-      </c>
-      <c r="DH7" s="58"/>
+        <v>218.55135320950984</v>
+      </c>
+      <c r="DH7" s="58">
+        <v>225.51663585744626</v>
+      </c>
       <c r="DI7" s="58"/>
       <c r="DJ7" s="58"/>
       <c r="DK7" s="58"/>
@@ -7305,9 +7343,11 @@
         <v>67.851890272785425</v>
       </c>
       <c r="DG8" s="54">
-        <v>65.651561649040971</v>
-      </c>
-      <c r="DH8" s="54"/>
+        <v>66.462302515893384</v>
+      </c>
+      <c r="DH8" s="54">
+        <v>68.75978791081215</v>
+      </c>
       <c r="DI8" s="54"/>
       <c r="DJ8" s="54"/>
       <c r="DK8" s="54"/>
@@ -7730,9 +7770,11 @@
         <v>194.42439514079197</v>
       </c>
       <c r="DG9" s="58">
-        <v>196.13465958988701</v>
-      </c>
-      <c r="DH9" s="58"/>
+        <v>188.7688292894635</v>
+      </c>
+      <c r="DH9" s="58">
+        <v>193.27463559463283</v>
+      </c>
       <c r="DI9" s="58"/>
       <c r="DJ9" s="58"/>
       <c r="DK9" s="58"/>
@@ -8155,9 +8197,11 @@
         <v>126.92950949907261</v>
       </c>
       <c r="DG10" s="54">
-        <v>126.0802989675648</v>
-      </c>
-      <c r="DH10" s="54"/>
+        <v>124.40713827323454</v>
+      </c>
+      <c r="DH10" s="54">
+        <v>127.6866887997507</v>
+      </c>
       <c r="DI10" s="54"/>
       <c r="DJ10" s="54"/>
       <c r="DK10" s="54"/>
@@ -8580,9 +8624,11 @@
         <v>62.045991199586382</v>
       </c>
       <c r="DG11" s="58">
-        <v>58.497348837423708</v>
-      </c>
-      <c r="DH11" s="58"/>
+        <v>56.693929668280653</v>
+      </c>
+      <c r="DH11" s="58">
+        <v>58.128317388503504</v>
+      </c>
       <c r="DI11" s="58"/>
       <c r="DJ11" s="58"/>
       <c r="DK11" s="58"/>
@@ -9005,9 +9051,11 @@
         <v>81.767483423105062</v>
       </c>
       <c r="DG12" s="54">
-        <v>78.958526933561387</v>
-      </c>
-      <c r="DH12" s="54"/>
+        <v>73.491611816327335</v>
+      </c>
+      <c r="DH12" s="54">
+        <v>76.276082555986548</v>
+      </c>
       <c r="DI12" s="54"/>
       <c r="DJ12" s="54"/>
       <c r="DK12" s="54"/>
@@ -9430,9 +9478,11 @@
         <v>70.67189567895899</v>
       </c>
       <c r="DG13" s="58">
-        <v>65.434962189046558</v>
-      </c>
-      <c r="DH13" s="58"/>
+        <v>64.499344667970234</v>
+      </c>
+      <c r="DH13" s="58">
+        <v>65.846206767340533</v>
+      </c>
       <c r="DI13" s="58"/>
       <c r="DJ13" s="58"/>
       <c r="DK13" s="58"/>
@@ -9855,9 +9905,11 @@
         <v>181.96736269002298</v>
       </c>
       <c r="DG14" s="115">
-        <v>180.64884227133069</v>
-      </c>
-      <c r="DH14" s="115"/>
+        <v>177.125176043339</v>
+      </c>
+      <c r="DH14" s="115">
+        <v>182.33178176823262</v>
+      </c>
       <c r="DI14" s="115"/>
       <c r="DJ14" s="115"/>
       <c r="DK14" s="115"/>
@@ -10162,7 +10214,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BJ6" sqref="BJ6:DR14"/>
+      <selection pane="topRight" activeCell="BJ6" sqref="BJ6:DH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -10178,8 +10230,8 @@
     <col min="79" max="79" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="80" max="100" width="7" customWidth="1"/>
     <col min="101" max="101" width="7.08984375" customWidth="1"/>
-    <col min="102" max="111" width="7" customWidth="1"/>
-    <col min="112" max="121" width="7" hidden="1" customWidth="1"/>
+    <col min="102" max="112" width="7" customWidth="1"/>
+    <col min="113" max="121" width="7" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="45.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10345,155 +10397,155 @@
       <c r="BX3" s="3"/>
     </row>
     <row r="4" spans="1:124" ht="18" customHeight="1">
-      <c r="A4" s="138" t="s">
+      <c r="A4" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="M4" s="141"/>
-      <c r="N4" s="144">
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="145">
         <v>2013</v>
       </c>
-      <c r="O4" s="141"/>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="141"/>
-      <c r="R4" s="141"/>
-      <c r="S4" s="141"/>
-      <c r="T4" s="141"/>
-      <c r="U4" s="141"/>
-      <c r="V4" s="141"/>
-      <c r="W4" s="141"/>
-      <c r="X4" s="141"/>
-      <c r="Y4" s="141"/>
-      <c r="Z4" s="144">
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
+      <c r="Q4" s="142"/>
+      <c r="R4" s="142"/>
+      <c r="S4" s="142"/>
+      <c r="T4" s="142"/>
+      <c r="U4" s="142"/>
+      <c r="V4" s="142"/>
+      <c r="W4" s="142"/>
+      <c r="X4" s="142"/>
+      <c r="Y4" s="142"/>
+      <c r="Z4" s="145">
         <v>2014</v>
       </c>
-      <c r="AA4" s="141"/>
-      <c r="AB4" s="141"/>
-      <c r="AC4" s="141"/>
-      <c r="AD4" s="141"/>
-      <c r="AE4" s="141"/>
-      <c r="AF4" s="141"/>
-      <c r="AG4" s="141"/>
-      <c r="AH4" s="141"/>
-      <c r="AI4" s="141"/>
-      <c r="AJ4" s="141"/>
-      <c r="AK4" s="141"/>
-      <c r="AL4" s="144">
+      <c r="AA4" s="142"/>
+      <c r="AB4" s="142"/>
+      <c r="AC4" s="142"/>
+      <c r="AD4" s="142"/>
+      <c r="AE4" s="142"/>
+      <c r="AF4" s="142"/>
+      <c r="AG4" s="142"/>
+      <c r="AH4" s="142"/>
+      <c r="AI4" s="142"/>
+      <c r="AJ4" s="142"/>
+      <c r="AK4" s="142"/>
+      <c r="AL4" s="145">
         <v>2015</v>
       </c>
-      <c r="AM4" s="141"/>
-      <c r="AN4" s="141"/>
-      <c r="AO4" s="141"/>
-      <c r="AP4" s="141"/>
-      <c r="AQ4" s="141"/>
-      <c r="AR4" s="141"/>
-      <c r="AS4" s="141"/>
-      <c r="AT4" s="141"/>
-      <c r="AU4" s="141"/>
-      <c r="AV4" s="141"/>
-      <c r="AW4" s="141"/>
-      <c r="AX4" s="144">
+      <c r="AM4" s="142"/>
+      <c r="AN4" s="142"/>
+      <c r="AO4" s="142"/>
+      <c r="AP4" s="142"/>
+      <c r="AQ4" s="142"/>
+      <c r="AR4" s="142"/>
+      <c r="AS4" s="142"/>
+      <c r="AT4" s="142"/>
+      <c r="AU4" s="142"/>
+      <c r="AV4" s="142"/>
+      <c r="AW4" s="142"/>
+      <c r="AX4" s="145">
         <v>2016</v>
       </c>
-      <c r="AY4" s="141"/>
-      <c r="AZ4" s="141"/>
-      <c r="BA4" s="141"/>
-      <c r="BB4" s="141"/>
-      <c r="BC4" s="141"/>
-      <c r="BD4" s="141"/>
-      <c r="BE4" s="141"/>
-      <c r="BF4" s="141"/>
-      <c r="BG4" s="141"/>
-      <c r="BH4" s="141"/>
-      <c r="BI4" s="141"/>
-      <c r="BJ4" s="144">
+      <c r="AY4" s="142"/>
+      <c r="AZ4" s="142"/>
+      <c r="BA4" s="142"/>
+      <c r="BB4" s="142"/>
+      <c r="BC4" s="142"/>
+      <c r="BD4" s="142"/>
+      <c r="BE4" s="142"/>
+      <c r="BF4" s="142"/>
+      <c r="BG4" s="142"/>
+      <c r="BH4" s="142"/>
+      <c r="BI4" s="142"/>
+      <c r="BJ4" s="145">
         <v>2017</v>
       </c>
-      <c r="BK4" s="141"/>
-      <c r="BL4" s="141"/>
-      <c r="BM4" s="141"/>
-      <c r="BN4" s="141"/>
-      <c r="BO4" s="141"/>
-      <c r="BP4" s="141"/>
-      <c r="BQ4" s="141"/>
-      <c r="BR4" s="141"/>
-      <c r="BS4" s="141"/>
-      <c r="BT4" s="141"/>
-      <c r="BU4" s="141"/>
-      <c r="BV4" s="144">
+      <c r="BK4" s="142"/>
+      <c r="BL4" s="142"/>
+      <c r="BM4" s="142"/>
+      <c r="BN4" s="142"/>
+      <c r="BO4" s="142"/>
+      <c r="BP4" s="142"/>
+      <c r="BQ4" s="142"/>
+      <c r="BR4" s="142"/>
+      <c r="BS4" s="142"/>
+      <c r="BT4" s="142"/>
+      <c r="BU4" s="142"/>
+      <c r="BV4" s="145">
         <v>2018</v>
       </c>
-      <c r="BW4" s="141"/>
-      <c r="BX4" s="141"/>
-      <c r="BY4" s="141"/>
-      <c r="BZ4" s="141"/>
-      <c r="CA4" s="141"/>
-      <c r="CB4" s="141"/>
-      <c r="CC4" s="141"/>
-      <c r="CD4" s="145"/>
-      <c r="CE4" s="141"/>
-      <c r="CF4" s="141"/>
-      <c r="CG4" s="141"/>
-      <c r="CH4" s="144">
+      <c r="BW4" s="142"/>
+      <c r="BX4" s="142"/>
+      <c r="BY4" s="142"/>
+      <c r="BZ4" s="142"/>
+      <c r="CA4" s="142"/>
+      <c r="CB4" s="142"/>
+      <c r="CC4" s="142"/>
+      <c r="CD4" s="146"/>
+      <c r="CE4" s="142"/>
+      <c r="CF4" s="142"/>
+      <c r="CG4" s="142"/>
+      <c r="CH4" s="145">
         <v>2019</v>
       </c>
-      <c r="CI4" s="141"/>
-      <c r="CJ4" s="141"/>
-      <c r="CK4" s="141"/>
-      <c r="CL4" s="141"/>
-      <c r="CM4" s="141"/>
-      <c r="CN4" s="141"/>
-      <c r="CO4" s="141"/>
-      <c r="CP4" s="145"/>
-      <c r="CQ4" s="141"/>
-      <c r="CR4" s="141"/>
-      <c r="CS4" s="141"/>
-      <c r="CT4" s="144">
+      <c r="CI4" s="142"/>
+      <c r="CJ4" s="142"/>
+      <c r="CK4" s="142"/>
+      <c r="CL4" s="142"/>
+      <c r="CM4" s="142"/>
+      <c r="CN4" s="142"/>
+      <c r="CO4" s="142"/>
+      <c r="CP4" s="146"/>
+      <c r="CQ4" s="142"/>
+      <c r="CR4" s="142"/>
+      <c r="CS4" s="142"/>
+      <c r="CT4" s="145">
         <v>2020</v>
       </c>
-      <c r="CU4" s="141"/>
-      <c r="CV4" s="141"/>
-      <c r="CW4" s="141"/>
-      <c r="CX4" s="141"/>
-      <c r="CY4" s="141"/>
-      <c r="CZ4" s="141"/>
-      <c r="DA4" s="141"/>
-      <c r="DB4" s="145"/>
-      <c r="DC4" s="141"/>
-      <c r="DD4" s="141"/>
-      <c r="DE4" s="141"/>
-      <c r="DF4" s="144">
+      <c r="CU4" s="142"/>
+      <c r="CV4" s="142"/>
+      <c r="CW4" s="142"/>
+      <c r="CX4" s="142"/>
+      <c r="CY4" s="142"/>
+      <c r="CZ4" s="142"/>
+      <c r="DA4" s="142"/>
+      <c r="DB4" s="146"/>
+      <c r="DC4" s="142"/>
+      <c r="DD4" s="142"/>
+      <c r="DE4" s="142"/>
+      <c r="DF4" s="145">
         <v>2021</v>
       </c>
-      <c r="DG4" s="141"/>
-      <c r="DH4" s="141"/>
-      <c r="DI4" s="141"/>
-      <c r="DJ4" s="141"/>
-      <c r="DK4" s="141"/>
-      <c r="DL4" s="141"/>
-      <c r="DM4" s="141"/>
-      <c r="DN4" s="145"/>
-      <c r="DO4" s="141"/>
-      <c r="DP4" s="141"/>
-      <c r="DQ4" s="141"/>
-      <c r="DR4" s="146" t="s">
+      <c r="DG4" s="142"/>
+      <c r="DH4" s="142"/>
+      <c r="DI4" s="142"/>
+      <c r="DJ4" s="142"/>
+      <c r="DK4" s="142"/>
+      <c r="DL4" s="142"/>
+      <c r="DM4" s="142"/>
+      <c r="DN4" s="146"/>
+      <c r="DO4" s="142"/>
+      <c r="DP4" s="142"/>
+      <c r="DQ4" s="142"/>
+      <c r="DR4" s="147" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:124" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="139"/>
+      <c r="A5" s="140"/>
       <c r="B5" s="71" t="s">
         <v>2</v>
       </c>
@@ -10822,10 +10874,10 @@
         <v>2</v>
       </c>
       <c r="DG5" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="DH5" s="50" t="s">
         <v>104</v>
-      </c>
-      <c r="DH5" s="50" t="s">
-        <v>4</v>
       </c>
       <c r="DI5" s="50" t="s">
         <v>5</v>
@@ -10854,7 +10906,7 @@
       <c r="DQ5" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="DR5" s="143"/>
+      <c r="DR5" s="144"/>
     </row>
     <row r="6" spans="1:124" ht="18" customHeight="1">
       <c r="A6" s="69" t="s">
@@ -11236,9 +11288,11 @@
         <v>-22.123146198472483</v>
       </c>
       <c r="DG6" s="54">
-        <v>-19.731522818557352</v>
-      </c>
-      <c r="DH6" s="54"/>
+        <v>-20.972676727920174</v>
+      </c>
+      <c r="DH6" s="54">
+        <v>-13.378792623811009</v>
+      </c>
       <c r="DI6" s="54"/>
       <c r="DJ6" s="54"/>
       <c r="DK6" s="54"/>
@@ -11632,9 +11686,11 @@
         <v>-6.9667727776364643</v>
       </c>
       <c r="DG7" s="58">
-        <v>-8.3747729657303438</v>
-      </c>
-      <c r="DH7" s="58"/>
+        <v>-9.8442892761888885</v>
+      </c>
+      <c r="DH7" s="58">
+        <v>-12.567533740436517</v>
+      </c>
       <c r="DI7" s="58"/>
       <c r="DJ7" s="58"/>
       <c r="DK7" s="58"/>
@@ -12028,9 +12084,11 @@
         <v>-17.07413020784702</v>
       </c>
       <c r="DG8" s="54">
-        <v>-18.504815441095147</v>
-      </c>
-      <c r="DH8" s="54"/>
+        <v>-17.498419326303733</v>
+      </c>
+      <c r="DH8" s="54">
+        <v>-1.2256734940270064</v>
+      </c>
       <c r="DI8" s="54"/>
       <c r="DJ8" s="54"/>
       <c r="DK8" s="54"/>
@@ -12424,9 +12482,11 @@
         <v>-38.796939337480637</v>
       </c>
       <c r="DG9" s="58">
-        <v>-37.378839649497117</v>
-      </c>
-      <c r="DH9" s="58"/>
+        <v>-39.730575142458392</v>
+      </c>
+      <c r="DH9" s="58">
+        <v>-36.363028404390221</v>
+      </c>
       <c r="DI9" s="58"/>
       <c r="DJ9" s="58"/>
       <c r="DK9" s="58"/>
@@ -12820,9 +12880,11 @@
         <v>-25.824136583767142</v>
       </c>
       <c r="DG10" s="54">
-        <v>-26.398008070802575</v>
-      </c>
-      <c r="DH10" s="54"/>
+        <v>-27.374750360666823</v>
+      </c>
+      <c r="DH10" s="54">
+        <v>-22.900671067171658</v>
+      </c>
       <c r="DI10" s="54"/>
       <c r="DJ10" s="54"/>
       <c r="DK10" s="54"/>
@@ -13216,9 +13278,11 @@
         <v>-53.033993842159781</v>
       </c>
       <c r="DG11" s="58">
-        <v>-49.427551732707776</v>
-      </c>
-      <c r="DH11" s="58"/>
+        <v>-50.986653545837861</v>
+      </c>
+      <c r="DH11" s="58">
+        <v>-41.860209082547726</v>
+      </c>
       <c r="DI11" s="58"/>
       <c r="DJ11" s="58"/>
       <c r="DK11" s="58"/>
@@ -13612,9 +13676,11 @@
         <v>-44.483647199467292</v>
       </c>
       <c r="DG12" s="54">
-        <v>-39.984725671558728</v>
-      </c>
-      <c r="DH12" s="54"/>
+        <v>-44.140051552538992</v>
+      </c>
+      <c r="DH12" s="54">
+        <v>-26.192649977232406</v>
+      </c>
       <c r="DI12" s="54"/>
       <c r="DJ12" s="54"/>
       <c r="DK12" s="54"/>
@@ -14008,9 +14074,11 @@
         <v>-46.282880589036644</v>
       </c>
       <c r="DG13" s="58">
-        <v>-40.486538373678513</v>
-      </c>
-      <c r="DH13" s="58"/>
+        <v>-41.337487706798335</v>
+      </c>
+      <c r="DH13" s="58">
+        <v>-16.034502015836011</v>
+      </c>
       <c r="DI13" s="58"/>
       <c r="DJ13" s="58"/>
       <c r="DK13" s="58"/>
@@ -14404,9 +14472,11 @@
         <v>-16.351743828103054</v>
       </c>
       <c r="DG14" s="62">
-        <v>-16.504557664251422</v>
-      </c>
-      <c r="DH14" s="115"/>
+        <v>-18.133187367329214</v>
+      </c>
+      <c r="DH14" s="62">
+        <v>-17.083498111989883</v>
+      </c>
       <c r="DI14" s="115"/>
       <c r="DJ14" s="115"/>
       <c r="DK14" s="115"/>
@@ -14711,7 +14781,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BJ6" sqref="BJ6:DG14"/>
+      <selection pane="topRight" activeCell="BJ6" sqref="BJ6:DH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -14724,8 +14794,8 @@
     <col min="74" max="75" width="8.54296875" customWidth="1"/>
     <col min="76" max="76" width="8.6328125" customWidth="1"/>
     <col min="77" max="77" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="80" max="111" width="9.08984375" customWidth="1"/>
-    <col min="112" max="121" width="9.08984375" hidden="1" customWidth="1"/>
+    <col min="80" max="112" width="9.08984375" customWidth="1"/>
+    <col min="113" max="121" width="9.08984375" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="43.08984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14890,155 +14960,155 @@
       <c r="BX3" s="9"/>
     </row>
     <row r="4" spans="1:122" ht="18" customHeight="1">
-      <c r="A4" s="138" t="s">
+      <c r="A4" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="M4" s="141"/>
-      <c r="N4" s="144">
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="145">
         <v>2013</v>
       </c>
-      <c r="O4" s="141"/>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="141"/>
-      <c r="R4" s="141"/>
-      <c r="S4" s="141"/>
-      <c r="T4" s="141"/>
-      <c r="U4" s="141"/>
-      <c r="V4" s="141"/>
-      <c r="W4" s="141"/>
-      <c r="X4" s="141"/>
-      <c r="Y4" s="141"/>
-      <c r="Z4" s="144">
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
+      <c r="Q4" s="142"/>
+      <c r="R4" s="142"/>
+      <c r="S4" s="142"/>
+      <c r="T4" s="142"/>
+      <c r="U4" s="142"/>
+      <c r="V4" s="142"/>
+      <c r="W4" s="142"/>
+      <c r="X4" s="142"/>
+      <c r="Y4" s="142"/>
+      <c r="Z4" s="145">
         <v>2014</v>
       </c>
-      <c r="AA4" s="141"/>
-      <c r="AB4" s="141"/>
-      <c r="AC4" s="141"/>
-      <c r="AD4" s="141"/>
-      <c r="AE4" s="141"/>
-      <c r="AF4" s="141"/>
-      <c r="AG4" s="141"/>
-      <c r="AH4" s="141"/>
-      <c r="AI4" s="141"/>
-      <c r="AJ4" s="141"/>
-      <c r="AK4" s="141"/>
-      <c r="AL4" s="144">
+      <c r="AA4" s="142"/>
+      <c r="AB4" s="142"/>
+      <c r="AC4" s="142"/>
+      <c r="AD4" s="142"/>
+      <c r="AE4" s="142"/>
+      <c r="AF4" s="142"/>
+      <c r="AG4" s="142"/>
+      <c r="AH4" s="142"/>
+      <c r="AI4" s="142"/>
+      <c r="AJ4" s="142"/>
+      <c r="AK4" s="142"/>
+      <c r="AL4" s="145">
         <v>2015</v>
       </c>
-      <c r="AM4" s="141"/>
-      <c r="AN4" s="141"/>
-      <c r="AO4" s="141"/>
-      <c r="AP4" s="141"/>
-      <c r="AQ4" s="141"/>
-      <c r="AR4" s="141"/>
-      <c r="AS4" s="141"/>
-      <c r="AT4" s="141"/>
-      <c r="AU4" s="141"/>
-      <c r="AV4" s="141"/>
-      <c r="AW4" s="141"/>
-      <c r="AX4" s="144">
+      <c r="AM4" s="142"/>
+      <c r="AN4" s="142"/>
+      <c r="AO4" s="142"/>
+      <c r="AP4" s="142"/>
+      <c r="AQ4" s="142"/>
+      <c r="AR4" s="142"/>
+      <c r="AS4" s="142"/>
+      <c r="AT4" s="142"/>
+      <c r="AU4" s="142"/>
+      <c r="AV4" s="142"/>
+      <c r="AW4" s="142"/>
+      <c r="AX4" s="145">
         <v>2016</v>
       </c>
-      <c r="AY4" s="141"/>
-      <c r="AZ4" s="141"/>
-      <c r="BA4" s="141"/>
-      <c r="BB4" s="141"/>
-      <c r="BC4" s="141"/>
-      <c r="BD4" s="141"/>
-      <c r="BE4" s="141"/>
-      <c r="BF4" s="141"/>
-      <c r="BG4" s="141"/>
-      <c r="BH4" s="141"/>
-      <c r="BI4" s="141"/>
-      <c r="BJ4" s="144">
+      <c r="AY4" s="142"/>
+      <c r="AZ4" s="142"/>
+      <c r="BA4" s="142"/>
+      <c r="BB4" s="142"/>
+      <c r="BC4" s="142"/>
+      <c r="BD4" s="142"/>
+      <c r="BE4" s="142"/>
+      <c r="BF4" s="142"/>
+      <c r="BG4" s="142"/>
+      <c r="BH4" s="142"/>
+      <c r="BI4" s="142"/>
+      <c r="BJ4" s="145">
         <v>2017</v>
       </c>
-      <c r="BK4" s="141"/>
-      <c r="BL4" s="141"/>
-      <c r="BM4" s="141"/>
-      <c r="BN4" s="141"/>
-      <c r="BO4" s="141"/>
-      <c r="BP4" s="141"/>
-      <c r="BQ4" s="141"/>
-      <c r="BR4" s="141"/>
-      <c r="BS4" s="141"/>
-      <c r="BT4" s="141"/>
-      <c r="BU4" s="141"/>
-      <c r="BV4" s="144">
+      <c r="BK4" s="142"/>
+      <c r="BL4" s="142"/>
+      <c r="BM4" s="142"/>
+      <c r="BN4" s="142"/>
+      <c r="BO4" s="142"/>
+      <c r="BP4" s="142"/>
+      <c r="BQ4" s="142"/>
+      <c r="BR4" s="142"/>
+      <c r="BS4" s="142"/>
+      <c r="BT4" s="142"/>
+      <c r="BU4" s="142"/>
+      <c r="BV4" s="145">
         <v>2018</v>
       </c>
-      <c r="BW4" s="141"/>
-      <c r="BX4" s="141"/>
-      <c r="BY4" s="141"/>
-      <c r="BZ4" s="141"/>
-      <c r="CA4" s="141"/>
-      <c r="CB4" s="141"/>
-      <c r="CC4" s="141"/>
-      <c r="CD4" s="145"/>
-      <c r="CE4" s="141"/>
-      <c r="CF4" s="141"/>
-      <c r="CG4" s="141"/>
-      <c r="CH4" s="144">
+      <c r="BW4" s="142"/>
+      <c r="BX4" s="142"/>
+      <c r="BY4" s="142"/>
+      <c r="BZ4" s="142"/>
+      <c r="CA4" s="142"/>
+      <c r="CB4" s="142"/>
+      <c r="CC4" s="142"/>
+      <c r="CD4" s="146"/>
+      <c r="CE4" s="142"/>
+      <c r="CF4" s="142"/>
+      <c r="CG4" s="142"/>
+      <c r="CH4" s="145">
         <v>2019</v>
       </c>
-      <c r="CI4" s="141"/>
-      <c r="CJ4" s="141"/>
-      <c r="CK4" s="141"/>
-      <c r="CL4" s="141"/>
-      <c r="CM4" s="141"/>
-      <c r="CN4" s="141"/>
-      <c r="CO4" s="141"/>
-      <c r="CP4" s="145"/>
-      <c r="CQ4" s="141"/>
-      <c r="CR4" s="141"/>
-      <c r="CS4" s="141"/>
-      <c r="CT4" s="144">
+      <c r="CI4" s="142"/>
+      <c r="CJ4" s="142"/>
+      <c r="CK4" s="142"/>
+      <c r="CL4" s="142"/>
+      <c r="CM4" s="142"/>
+      <c r="CN4" s="142"/>
+      <c r="CO4" s="142"/>
+      <c r="CP4" s="146"/>
+      <c r="CQ4" s="142"/>
+      <c r="CR4" s="142"/>
+      <c r="CS4" s="142"/>
+      <c r="CT4" s="145">
         <v>2020</v>
       </c>
-      <c r="CU4" s="141"/>
-      <c r="CV4" s="141"/>
-      <c r="CW4" s="141"/>
-      <c r="CX4" s="141"/>
-      <c r="CY4" s="141"/>
-      <c r="CZ4" s="141"/>
-      <c r="DA4" s="141"/>
-      <c r="DB4" s="145"/>
-      <c r="DC4" s="141"/>
-      <c r="DD4" s="141"/>
-      <c r="DE4" s="141"/>
-      <c r="DF4" s="144">
+      <c r="CU4" s="142"/>
+      <c r="CV4" s="142"/>
+      <c r="CW4" s="142"/>
+      <c r="CX4" s="142"/>
+      <c r="CY4" s="142"/>
+      <c r="CZ4" s="142"/>
+      <c r="DA4" s="142"/>
+      <c r="DB4" s="146"/>
+      <c r="DC4" s="142"/>
+      <c r="DD4" s="142"/>
+      <c r="DE4" s="142"/>
+      <c r="DF4" s="145">
         <v>2021</v>
       </c>
-      <c r="DG4" s="141"/>
-      <c r="DH4" s="141"/>
-      <c r="DI4" s="141"/>
-      <c r="DJ4" s="141"/>
-      <c r="DK4" s="141"/>
-      <c r="DL4" s="141"/>
-      <c r="DM4" s="141"/>
-      <c r="DN4" s="145"/>
-      <c r="DO4" s="141"/>
-      <c r="DP4" s="141"/>
-      <c r="DQ4" s="141"/>
-      <c r="DR4" s="146" t="s">
+      <c r="DG4" s="142"/>
+      <c r="DH4" s="142"/>
+      <c r="DI4" s="142"/>
+      <c r="DJ4" s="142"/>
+      <c r="DK4" s="142"/>
+      <c r="DL4" s="142"/>
+      <c r="DM4" s="142"/>
+      <c r="DN4" s="146"/>
+      <c r="DO4" s="142"/>
+      <c r="DP4" s="142"/>
+      <c r="DQ4" s="142"/>
+      <c r="DR4" s="147" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:122" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="139"/>
+      <c r="A5" s="140"/>
       <c r="B5" s="71" t="s">
         <v>2</v>
       </c>
@@ -15367,10 +15437,10 @@
         <v>2</v>
       </c>
       <c r="DG5" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="DH5" s="50" t="s">
         <v>104</v>
-      </c>
-      <c r="DH5" s="50" t="s">
-        <v>4</v>
       </c>
       <c r="DI5" s="50" t="s">
         <v>5</v>
@@ -15399,7 +15469,7 @@
       <c r="DQ5" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="DR5" s="143"/>
+      <c r="DR5" s="144"/>
     </row>
     <row r="6" spans="1:122" ht="18" customHeight="1">
       <c r="A6" s="69" t="s">
@@ -15792,9 +15862,11 @@
         <v>-4.9602402516912605</v>
       </c>
       <c r="DG6" s="54">
-        <v>0.44728192673117917</v>
-      </c>
-      <c r="DH6" s="54"/>
+        <v>-1.1058873998329659</v>
+      </c>
+      <c r="DH6" s="54">
+        <v>-0.15153264276639788</v>
+      </c>
       <c r="DI6" s="54"/>
       <c r="DJ6" s="54"/>
       <c r="DK6" s="54"/>
@@ -16199,9 +16271,11 @@
         <v>-3.5512012377250812</v>
       </c>
       <c r="DG7" s="58">
-        <v>-0.79947632771194321</v>
-      </c>
-      <c r="DH7" s="58"/>
+        <v>-2.3904878019638147</v>
+      </c>
+      <c r="DH7" s="58">
+        <v>3.1870233451537047</v>
+      </c>
       <c r="DI7" s="58"/>
       <c r="DJ7" s="58"/>
       <c r="DK7" s="58"/>
@@ -16606,9 +16680,11 @@
         <v>-10.389873278954553</v>
       </c>
       <c r="DG8" s="54">
-        <v>-3.2428405677402026</v>
-      </c>
-      <c r="DH8" s="54"/>
+        <v>-2.0479720628349014</v>
+      </c>
+      <c r="DH8" s="54">
+        <v>3.4568248585269146</v>
+      </c>
       <c r="DI8" s="54"/>
       <c r="DJ8" s="54"/>
       <c r="DK8" s="54"/>
@@ -17013,9 +17089,11 @@
         <v>-5.6633515134262638</v>
       </c>
       <c r="DG9" s="58">
-        <v>0.87965527569548385</v>
-      </c>
-      <c r="DH9" s="58"/>
+        <v>-2.9088766598620595</v>
+      </c>
+      <c r="DH9" s="58">
+        <v>2.3869440320891044</v>
+      </c>
       <c r="DI9" s="58"/>
       <c r="DJ9" s="58"/>
       <c r="DK9" s="58"/>
@@ -17420,9 +17498,11 @@
         <v>-6.9245550929385473</v>
       </c>
       <c r="DG10" s="54">
-        <v>-0.66904105661419067</v>
-      </c>
-      <c r="DH10" s="54"/>
+        <v>-1.9872220697870802</v>
+      </c>
+      <c r="DH10" s="54">
+        <v>2.6361433692922986</v>
+      </c>
       <c r="DI10" s="54"/>
       <c r="DJ10" s="54"/>
       <c r="DK10" s="54"/>
@@ -17827,9 +17907,11 @@
         <v>-4.2042464522516667</v>
       </c>
       <c r="DG11" s="58">
-        <v>-5.7193741183819213</v>
-      </c>
-      <c r="DH11" s="58"/>
+        <v>-8.6259586281561553</v>
+      </c>
+      <c r="DH11" s="58">
+        <v>2.5300552080540655</v>
+      </c>
       <c r="DI11" s="58"/>
       <c r="DJ11" s="58"/>
       <c r="DK11" s="58"/>
@@ -18234,9 +18316,11 @@
         <v>-3.9183192496097377</v>
       </c>
       <c r="DG12" s="54">
-        <v>-3.4352977148737125</v>
-      </c>
-      <c r="DH12" s="54"/>
+        <v>-10.121225773764252</v>
+      </c>
+      <c r="DH12" s="54">
+        <v>3.7888279639562796</v>
+      </c>
       <c r="DI12" s="54"/>
       <c r="DJ12" s="54"/>
       <c r="DK12" s="54"/>
@@ -18641,9 +18725,11 @@
         <v>-7.1509825759810894</v>
       </c>
       <c r="DG13" s="58">
-        <v>-7.4102066169304948</v>
-      </c>
-      <c r="DH13" s="58"/>
+        <v>-8.7340957132787054</v>
+      </c>
+      <c r="DH13" s="58">
+        <v>2.0881795098906366</v>
+      </c>
       <c r="DI13" s="58"/>
       <c r="DJ13" s="58"/>
       <c r="DK13" s="58"/>
@@ -19048,9 +19134,11 @@
         <v>-4.2571274409940827</v>
       </c>
       <c r="DG14" s="62">
-        <v>-0.72459170655693583</v>
-      </c>
-      <c r="DH14" s="115"/>
+        <v>-2.6610193031881977</v>
+      </c>
+      <c r="DH14" s="62">
+        <v>2.9395063091537423</v>
+      </c>
       <c r="DI14" s="115"/>
       <c r="DJ14" s="115"/>
       <c r="DK14" s="115"/>
@@ -19352,7 +19440,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V6" sqref="V6:AK14"/>
+      <selection pane="topRight" activeCell="V6" sqref="V6:AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -19361,8 +19449,8 @@
     <col min="2" max="21" width="8.90625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="22" max="22" width="9.08984375" collapsed="1"/>
     <col min="24" max="25" width="8.08984375" customWidth="1"/>
-    <col min="26" max="37" width="7.54296875" style="48" customWidth="1"/>
-    <col min="38" max="41" width="7.54296875" style="48" hidden="1" customWidth="1"/>
+    <col min="26" max="38" width="7.54296875" style="48" customWidth="1"/>
+    <col min="39" max="41" width="7.54296875" style="48" hidden="1" customWidth="1"/>
     <col min="42" max="42" width="43.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19458,75 +19546,75 @@
       <c r="AO3" s="46"/>
     </row>
     <row r="4" spans="1:42" ht="18" customHeight="1">
-      <c r="A4" s="138" t="s">
+      <c r="A4" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="150">
+      <c r="B4" s="151">
         <v>2012</v>
       </c>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="148">
+      <c r="C4" s="149"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="149">
         <v>2013</v>
       </c>
-      <c r="G4" s="148"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="149"/>
-      <c r="J4" s="148">
+      <c r="G4" s="149"/>
+      <c r="H4" s="149"/>
+      <c r="I4" s="150"/>
+      <c r="J4" s="149">
         <v>2014</v>
       </c>
-      <c r="K4" s="148"/>
-      <c r="L4" s="148"/>
-      <c r="M4" s="149"/>
-      <c r="N4" s="148">
+      <c r="K4" s="149"/>
+      <c r="L4" s="149"/>
+      <c r="M4" s="150"/>
+      <c r="N4" s="149">
         <v>2015</v>
       </c>
-      <c r="O4" s="148"/>
-      <c r="P4" s="148"/>
-      <c r="Q4" s="149"/>
-      <c r="R4" s="148">
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="150"/>
+      <c r="R4" s="149">
         <v>2016</v>
       </c>
-      <c r="S4" s="148"/>
-      <c r="T4" s="148"/>
-      <c r="U4" s="149"/>
-      <c r="V4" s="148">
+      <c r="S4" s="149"/>
+      <c r="T4" s="149"/>
+      <c r="U4" s="150"/>
+      <c r="V4" s="149">
         <v>2017</v>
       </c>
-      <c r="W4" s="148"/>
-      <c r="X4" s="148"/>
-      <c r="Y4" s="149"/>
-      <c r="Z4" s="148">
+      <c r="W4" s="149"/>
+      <c r="X4" s="149"/>
+      <c r="Y4" s="150"/>
+      <c r="Z4" s="149">
         <v>2018</v>
       </c>
-      <c r="AA4" s="148"/>
-      <c r="AB4" s="148"/>
-      <c r="AC4" s="149"/>
-      <c r="AD4" s="148">
+      <c r="AA4" s="149"/>
+      <c r="AB4" s="149"/>
+      <c r="AC4" s="150"/>
+      <c r="AD4" s="149">
         <v>2019</v>
       </c>
-      <c r="AE4" s="148"/>
-      <c r="AF4" s="148"/>
-      <c r="AG4" s="149"/>
-      <c r="AH4" s="148">
+      <c r="AE4" s="149"/>
+      <c r="AF4" s="149"/>
+      <c r="AG4" s="150"/>
+      <c r="AH4" s="149">
         <v>2020</v>
       </c>
-      <c r="AI4" s="148"/>
-      <c r="AJ4" s="148"/>
-      <c r="AK4" s="149"/>
-      <c r="AL4" s="148">
+      <c r="AI4" s="149"/>
+      <c r="AJ4" s="149"/>
+      <c r="AK4" s="150"/>
+      <c r="AL4" s="149">
         <v>2021</v>
       </c>
-      <c r="AM4" s="148"/>
-      <c r="AN4" s="148"/>
-      <c r="AO4" s="149"/>
-      <c r="AP4" s="142" t="s">
+      <c r="AM4" s="149"/>
+      <c r="AN4" s="149"/>
+      <c r="AO4" s="150"/>
+      <c r="AP4" s="143" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:42" ht="18" customHeight="1">
-      <c r="A5" s="139"/>
+      <c r="A5" s="140"/>
       <c r="B5" s="75" t="s">
         <v>32</v>
       </c>
@@ -19636,7 +19724,7 @@
         <v>35</v>
       </c>
       <c r="AL5" s="76" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="AM5" s="76" t="s">
         <v>33</v>
@@ -19647,7 +19735,7 @@
       <c r="AO5" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="AP5" s="147"/>
+      <c r="AP5" s="148"/>
     </row>
     <row r="6" spans="1:42" ht="18" customHeight="1">
       <c r="A6" s="69" t="s">
@@ -19781,7 +19869,9 @@
       <c r="AK6" s="55">
         <v>-21.483971839408341</v>
       </c>
-      <c r="AL6" s="54"/>
+      <c r="AL6" s="54">
+        <v>-18.82487185006789</v>
+      </c>
       <c r="AM6" s="54"/>
       <c r="AN6" s="54"/>
       <c r="AO6" s="54"/>
@@ -19921,7 +20011,9 @@
       <c r="AK7" s="59">
         <v>-7.4748951418588065</v>
       </c>
-      <c r="AL7" s="58"/>
+      <c r="AL7" s="58">
+        <v>-9.7928652647539547</v>
+      </c>
       <c r="AM7" s="58"/>
       <c r="AN7" s="58"/>
       <c r="AO7" s="58"/>
@@ -20061,7 +20153,9 @@
       <c r="AK8" s="55">
         <v>-14.502101997089889</v>
       </c>
-      <c r="AL8" s="54"/>
+      <c r="AL8" s="54">
+        <v>-11.932741009392585</v>
+      </c>
       <c r="AM8" s="54"/>
       <c r="AN8" s="54"/>
       <c r="AO8" s="54"/>
@@ -20201,7 +20295,9 @@
       <c r="AK9" s="59">
         <v>-35.447976949969863</v>
       </c>
-      <c r="AL9" s="58"/>
+      <c r="AL9" s="58">
+        <v>-38.296847628109752</v>
+      </c>
       <c r="AM9" s="58"/>
       <c r="AN9" s="58"/>
       <c r="AO9" s="58"/>
@@ -20341,7 +20437,9 @@
       <c r="AK10" s="55">
         <v>-24.893164418499669</v>
       </c>
-      <c r="AL10" s="54"/>
+      <c r="AL10" s="54">
+        <v>-25.366519337201879</v>
+      </c>
       <c r="AM10" s="54"/>
       <c r="AN10" s="54"/>
       <c r="AO10" s="54"/>
@@ -20481,7 +20579,9 @@
       <c r="AK11" s="59">
         <v>-40.312947524790644</v>
       </c>
-      <c r="AL11" s="58"/>
+      <c r="AL11" s="58">
+        <v>-48.626952156848461</v>
+      </c>
       <c r="AM11" s="58"/>
       <c r="AN11" s="58"/>
       <c r="AO11" s="58"/>
@@ -20621,7 +20721,9 @@
       <c r="AK12" s="55">
         <v>-53.275949027343387</v>
       </c>
-      <c r="AL12" s="54"/>
+      <c r="AL12" s="54">
+        <v>-38.272116243079559</v>
+      </c>
       <c r="AM12" s="54"/>
       <c r="AN12" s="54"/>
       <c r="AO12" s="54"/>
@@ -20761,7 +20863,9 @@
       <c r="AK13" s="59">
         <v>-58.119154074942578</v>
       </c>
-      <c r="AL13" s="58"/>
+      <c r="AL13" s="58">
+        <v>-34.551623437223661</v>
+      </c>
       <c r="AM13" s="58"/>
       <c r="AN13" s="58"/>
       <c r="AO13" s="58"/>
@@ -20901,7 +21005,9 @@
       <c r="AK14" s="116">
         <v>-16.792045380275134</v>
       </c>
-      <c r="AL14" s="123"/>
+      <c r="AL14" s="123">
+        <v>-17.189476435807389</v>
+      </c>
       <c r="AM14" s="123"/>
       <c r="AN14" s="123"/>
       <c r="AO14" s="123"/>
@@ -21171,10 +21277,10 @@
   <dimension ref="A2:FD22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="BJ6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="DC6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BJ6" sqref="BJ6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -21185,30 +21291,30 @@
     <col min="62" max="62" width="9.36328125" customWidth="1" collapsed="1"/>
     <col min="63" max="91" width="9.36328125" customWidth="1"/>
     <col min="92" max="92" width="10.1796875" customWidth="1"/>
-    <col min="93" max="111" width="9.36328125" customWidth="1"/>
-    <col min="112" max="121" width="9.36328125" hidden="1" customWidth="1"/>
+    <col min="93" max="112" width="9.36328125" customWidth="1"/>
+    <col min="113" max="121" width="9.36328125" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="42.08984375" style="34" customWidth="1"/>
     <col min="125" max="125" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:160" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="155" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="154"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
+      <c r="L2" s="155"/>
+      <c r="M2" s="155"/>
+      <c r="N2" s="155"/>
+      <c r="O2" s="155"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -21481,155 +21587,155 @@
       <c r="DQ3" s="3"/>
     </row>
     <row r="4" spans="1:160" ht="18" customHeight="1">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="M4" s="141"/>
-      <c r="N4" s="144">
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="145">
         <v>2013</v>
       </c>
-      <c r="O4" s="141"/>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="141"/>
-      <c r="R4" s="141"/>
-      <c r="S4" s="141"/>
-      <c r="T4" s="141"/>
-      <c r="U4" s="141"/>
-      <c r="V4" s="141"/>
-      <c r="W4" s="141"/>
-      <c r="X4" s="141"/>
-      <c r="Y4" s="141"/>
-      <c r="Z4" s="144">
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
+      <c r="Q4" s="142"/>
+      <c r="R4" s="142"/>
+      <c r="S4" s="142"/>
+      <c r="T4" s="142"/>
+      <c r="U4" s="142"/>
+      <c r="V4" s="142"/>
+      <c r="W4" s="142"/>
+      <c r="X4" s="142"/>
+      <c r="Y4" s="142"/>
+      <c r="Z4" s="145">
         <v>2014</v>
       </c>
-      <c r="AA4" s="141"/>
-      <c r="AB4" s="141"/>
-      <c r="AC4" s="141"/>
-      <c r="AD4" s="141"/>
-      <c r="AE4" s="141"/>
-      <c r="AF4" s="141"/>
-      <c r="AG4" s="141"/>
-      <c r="AH4" s="141"/>
-      <c r="AI4" s="141"/>
-      <c r="AJ4" s="141"/>
-      <c r="AK4" s="141"/>
-      <c r="AL4" s="144">
+      <c r="AA4" s="142"/>
+      <c r="AB4" s="142"/>
+      <c r="AC4" s="142"/>
+      <c r="AD4" s="142"/>
+      <c r="AE4" s="142"/>
+      <c r="AF4" s="142"/>
+      <c r="AG4" s="142"/>
+      <c r="AH4" s="142"/>
+      <c r="AI4" s="142"/>
+      <c r="AJ4" s="142"/>
+      <c r="AK4" s="142"/>
+      <c r="AL4" s="145">
         <v>2015</v>
       </c>
-      <c r="AM4" s="141"/>
-      <c r="AN4" s="141"/>
-      <c r="AO4" s="141"/>
-      <c r="AP4" s="141"/>
-      <c r="AQ4" s="141"/>
-      <c r="AR4" s="141"/>
-      <c r="AS4" s="141"/>
-      <c r="AT4" s="141"/>
-      <c r="AU4" s="141"/>
-      <c r="AV4" s="141"/>
-      <c r="AW4" s="141"/>
-      <c r="AX4" s="144">
+      <c r="AM4" s="142"/>
+      <c r="AN4" s="142"/>
+      <c r="AO4" s="142"/>
+      <c r="AP4" s="142"/>
+      <c r="AQ4" s="142"/>
+      <c r="AR4" s="142"/>
+      <c r="AS4" s="142"/>
+      <c r="AT4" s="142"/>
+      <c r="AU4" s="142"/>
+      <c r="AV4" s="142"/>
+      <c r="AW4" s="142"/>
+      <c r="AX4" s="145">
         <v>2016</v>
       </c>
-      <c r="AY4" s="141"/>
-      <c r="AZ4" s="141"/>
-      <c r="BA4" s="141"/>
-      <c r="BB4" s="141"/>
-      <c r="BC4" s="141"/>
-      <c r="BD4" s="141"/>
-      <c r="BE4" s="141"/>
-      <c r="BF4" s="141"/>
-      <c r="BG4" s="141"/>
-      <c r="BH4" s="141"/>
-      <c r="BI4" s="141"/>
-      <c r="BJ4" s="144">
+      <c r="AY4" s="142"/>
+      <c r="AZ4" s="142"/>
+      <c r="BA4" s="142"/>
+      <c r="BB4" s="142"/>
+      <c r="BC4" s="142"/>
+      <c r="BD4" s="142"/>
+      <c r="BE4" s="142"/>
+      <c r="BF4" s="142"/>
+      <c r="BG4" s="142"/>
+      <c r="BH4" s="142"/>
+      <c r="BI4" s="142"/>
+      <c r="BJ4" s="145">
         <v>2017</v>
       </c>
-      <c r="BK4" s="141"/>
-      <c r="BL4" s="141"/>
-      <c r="BM4" s="141"/>
-      <c r="BN4" s="141"/>
-      <c r="BO4" s="141"/>
-      <c r="BP4" s="141"/>
-      <c r="BQ4" s="141"/>
-      <c r="BR4" s="141"/>
-      <c r="BS4" s="141"/>
-      <c r="BT4" s="141"/>
-      <c r="BU4" s="141"/>
-      <c r="BV4" s="144">
+      <c r="BK4" s="142"/>
+      <c r="BL4" s="142"/>
+      <c r="BM4" s="142"/>
+      <c r="BN4" s="142"/>
+      <c r="BO4" s="142"/>
+      <c r="BP4" s="142"/>
+      <c r="BQ4" s="142"/>
+      <c r="BR4" s="142"/>
+      <c r="BS4" s="142"/>
+      <c r="BT4" s="142"/>
+      <c r="BU4" s="142"/>
+      <c r="BV4" s="145">
         <v>2018</v>
       </c>
-      <c r="BW4" s="141"/>
-      <c r="BX4" s="141"/>
-      <c r="BY4" s="141"/>
-      <c r="BZ4" s="141"/>
-      <c r="CA4" s="141"/>
-      <c r="CB4" s="141"/>
-      <c r="CC4" s="141"/>
-      <c r="CD4" s="141"/>
-      <c r="CE4" s="141"/>
-      <c r="CF4" s="141"/>
-      <c r="CG4" s="141"/>
-      <c r="CH4" s="144">
+      <c r="BW4" s="142"/>
+      <c r="BX4" s="142"/>
+      <c r="BY4" s="142"/>
+      <c r="BZ4" s="142"/>
+      <c r="CA4" s="142"/>
+      <c r="CB4" s="142"/>
+      <c r="CC4" s="142"/>
+      <c r="CD4" s="142"/>
+      <c r="CE4" s="142"/>
+      <c r="CF4" s="142"/>
+      <c r="CG4" s="142"/>
+      <c r="CH4" s="145">
         <v>2019</v>
       </c>
-      <c r="CI4" s="141"/>
-      <c r="CJ4" s="141"/>
-      <c r="CK4" s="141"/>
-      <c r="CL4" s="141"/>
-      <c r="CM4" s="141"/>
-      <c r="CN4" s="141"/>
-      <c r="CO4" s="141"/>
-      <c r="CP4" s="141"/>
-      <c r="CQ4" s="141"/>
-      <c r="CR4" s="141"/>
-      <c r="CS4" s="141"/>
-      <c r="CT4" s="144">
+      <c r="CI4" s="142"/>
+      <c r="CJ4" s="142"/>
+      <c r="CK4" s="142"/>
+      <c r="CL4" s="142"/>
+      <c r="CM4" s="142"/>
+      <c r="CN4" s="142"/>
+      <c r="CO4" s="142"/>
+      <c r="CP4" s="142"/>
+      <c r="CQ4" s="142"/>
+      <c r="CR4" s="142"/>
+      <c r="CS4" s="142"/>
+      <c r="CT4" s="145">
         <v>2020</v>
       </c>
-      <c r="CU4" s="141"/>
-      <c r="CV4" s="141"/>
-      <c r="CW4" s="141"/>
-      <c r="CX4" s="141"/>
-      <c r="CY4" s="141"/>
-      <c r="CZ4" s="141"/>
-      <c r="DA4" s="141"/>
-      <c r="DB4" s="141"/>
-      <c r="DC4" s="141"/>
-      <c r="DD4" s="141"/>
-      <c r="DE4" s="141"/>
-      <c r="DF4" s="144">
+      <c r="CU4" s="142"/>
+      <c r="CV4" s="142"/>
+      <c r="CW4" s="142"/>
+      <c r="CX4" s="142"/>
+      <c r="CY4" s="142"/>
+      <c r="CZ4" s="142"/>
+      <c r="DA4" s="142"/>
+      <c r="DB4" s="142"/>
+      <c r="DC4" s="142"/>
+      <c r="DD4" s="142"/>
+      <c r="DE4" s="142"/>
+      <c r="DF4" s="145">
         <v>2021</v>
       </c>
-      <c r="DG4" s="141"/>
-      <c r="DH4" s="141"/>
-      <c r="DI4" s="141"/>
-      <c r="DJ4" s="141"/>
-      <c r="DK4" s="141"/>
-      <c r="DL4" s="141"/>
-      <c r="DM4" s="141"/>
-      <c r="DN4" s="145"/>
-      <c r="DO4" s="141"/>
-      <c r="DP4" s="141"/>
-      <c r="DQ4" s="141"/>
-      <c r="DR4" s="152" t="s">
+      <c r="DG4" s="142"/>
+      <c r="DH4" s="142"/>
+      <c r="DI4" s="142"/>
+      <c r="DJ4" s="142"/>
+      <c r="DK4" s="142"/>
+      <c r="DL4" s="142"/>
+      <c r="DM4" s="142"/>
+      <c r="DN4" s="146"/>
+      <c r="DO4" s="142"/>
+      <c r="DP4" s="142"/>
+      <c r="DQ4" s="142"/>
+      <c r="DR4" s="153" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:160" ht="18" customHeight="1">
-      <c r="A5" s="156"/>
+      <c r="A5" s="157"/>
       <c r="B5" s="50" t="s">
         <v>2</v>
       </c>
@@ -21958,10 +22064,10 @@
         <v>2</v>
       </c>
       <c r="DG5" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="DH5" s="50" t="s">
         <v>104</v>
-      </c>
-      <c r="DH5" s="50" t="s">
-        <v>4</v>
       </c>
       <c r="DI5" s="50" t="s">
         <v>5</v>
@@ -21990,7 +22096,7 @@
       <c r="DQ5" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="DR5" s="153"/>
+      <c r="DR5" s="154"/>
     </row>
     <row r="6" spans="1:160" ht="18" customHeight="1">
       <c r="A6" s="52" t="s">
@@ -22324,9 +22430,11 @@
         <v>55.27268474166646</v>
       </c>
       <c r="DG6" s="54">
-        <v>57.348154654466754</v>
-      </c>
-      <c r="DH6" s="54"/>
+        <v>56.674449853340398</v>
+      </c>
+      <c r="DH6" s="54">
+        <v>57.854872058599895</v>
+      </c>
       <c r="DI6" s="54"/>
       <c r="DJ6" s="54"/>
       <c r="DK6" s="54"/>
@@ -22672,9 +22780,11 @@
         <v>165.5021398912221</v>
       </c>
       <c r="DG7" s="58">
-        <v>164.05019005778905</v>
-      </c>
-      <c r="DH7" s="58"/>
+        <v>161.85810370999414</v>
+      </c>
+      <c r="DH7" s="58">
+        <v>161.24598392661505</v>
+      </c>
       <c r="DI7" s="58"/>
       <c r="DJ7" s="58"/>
       <c r="DK7" s="58"/>
@@ -23020,9 +23130,11 @@
         <v>304.79188452769949</v>
       </c>
       <c r="DG8" s="54">
-        <v>300.23671776436186</v>
-      </c>
-      <c r="DH8" s="54"/>
+        <v>299.62309780335374</v>
+      </c>
+      <c r="DH8" s="54">
+        <v>311.57467321328522</v>
+      </c>
       <c r="DI8" s="54"/>
       <c r="DJ8" s="54"/>
       <c r="DK8" s="54"/>
@@ -23368,9 +23480,11 @@
         <v>166.87089133193476</v>
       </c>
       <c r="DG9" s="58">
-        <v>166.87575717133907</v>
-      </c>
-      <c r="DH9" s="58"/>
+        <v>164.61598775448394</v>
+      </c>
+      <c r="DH9" s="58">
+        <v>166.14454941829396</v>
+      </c>
       <c r="DI9" s="58"/>
       <c r="DJ9" s="58"/>
       <c r="DK9" s="58"/>
@@ -23716,9 +23830,11 @@
         <v>106.9681416493802</v>
       </c>
       <c r="DG10" s="54">
-        <v>109.01832212943403</v>
-      </c>
-      <c r="DH10" s="54"/>
+        <v>98.50090515357941</v>
+      </c>
+      <c r="DH10" s="54">
+        <v>103.65938659998287</v>
+      </c>
       <c r="DI10" s="54"/>
       <c r="DJ10" s="54"/>
       <c r="DK10" s="54"/>
@@ -24064,9 +24180,11 @@
         <v>100.55157332113014</v>
       </c>
       <c r="DG11" s="58">
-        <v>94.548697017940199</v>
-      </c>
-      <c r="DH11" s="58"/>
+        <v>88.390756257908322</v>
+      </c>
+      <c r="DH11" s="58">
+        <v>100.29457995585365</v>
+      </c>
       <c r="DI11" s="58"/>
       <c r="DJ11" s="58"/>
       <c r="DK11" s="58"/>
@@ -24412,9 +24530,11 @@
         <v>173.9982198686715</v>
       </c>
       <c r="DG12" s="54">
-        <v>164.68797091348958</v>
-      </c>
-      <c r="DH12" s="54"/>
+        <v>161.95427108388122</v>
+      </c>
+      <c r="DH12" s="54">
+        <v>175.74348428526702</v>
+      </c>
       <c r="DI12" s="54"/>
       <c r="DJ12" s="54"/>
       <c r="DK12" s="54"/>
@@ -24760,9 +24880,11 @@
         <v>170.0627068729946</v>
       </c>
       <c r="DG13" s="58">
-        <v>172.10119929384871</v>
-      </c>
-      <c r="DH13" s="58"/>
+        <v>166.3982422575225</v>
+      </c>
+      <c r="DH13" s="58">
+        <v>159.69642631122898</v>
+      </c>
       <c r="DI13" s="58"/>
       <c r="DJ13" s="58"/>
       <c r="DK13" s="58"/>
@@ -25108,9 +25230,11 @@
         <v>89.782598308107069</v>
       </c>
       <c r="DG14" s="54">
-        <v>88.92520595453442</v>
-      </c>
-      <c r="DH14" s="54"/>
+        <v>87.96618315952675</v>
+      </c>
+      <c r="DH14" s="54">
+        <v>88.943509903933247</v>
+      </c>
       <c r="DI14" s="54"/>
       <c r="DJ14" s="54"/>
       <c r="DK14" s="54"/>
@@ -25456,9 +25580,11 @@
         <v>181.96736269002298</v>
       </c>
       <c r="DG15" s="115">
-        <v>180.64884227133069</v>
-      </c>
-      <c r="DH15" s="115"/>
+        <v>177.125176043339</v>
+      </c>
+      <c r="DH15" s="115">
+        <v>182.33178176823262</v>
+      </c>
       <c r="DI15" s="115"/>
       <c r="DJ15" s="115"/>
       <c r="DK15" s="115"/>
@@ -25963,7 +26089,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BJ6" sqref="BJ6:DG15"/>
+      <selection pane="topRight" activeCell="BJ6" sqref="BJ6:DH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -25974,8 +26100,8 @@
     <col min="74" max="75" width="8.6328125" customWidth="1"/>
     <col min="76" max="76" width="7.6328125" customWidth="1"/>
     <col min="77" max="77" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="80" max="111" width="9.08984375" customWidth="1"/>
-    <col min="112" max="121" width="9.08984375" hidden="1" customWidth="1"/>
+    <col min="80" max="112" width="9.08984375" customWidth="1"/>
+    <col min="113" max="121" width="9.08984375" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="28.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -26141,155 +26267,155 @@
       <c r="BX3" s="3"/>
     </row>
     <row r="4" spans="1:122" ht="18" customHeight="1">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="M4" s="141"/>
-      <c r="N4" s="144">
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="145">
         <v>2013</v>
       </c>
-      <c r="O4" s="141"/>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="141"/>
-      <c r="R4" s="141"/>
-      <c r="S4" s="141"/>
-      <c r="T4" s="141"/>
-      <c r="U4" s="141"/>
-      <c r="V4" s="141"/>
-      <c r="W4" s="141"/>
-      <c r="X4" s="141"/>
-      <c r="Y4" s="141"/>
-      <c r="Z4" s="144">
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
+      <c r="Q4" s="142"/>
+      <c r="R4" s="142"/>
+      <c r="S4" s="142"/>
+      <c r="T4" s="142"/>
+      <c r="U4" s="142"/>
+      <c r="V4" s="142"/>
+      <c r="W4" s="142"/>
+      <c r="X4" s="142"/>
+      <c r="Y4" s="142"/>
+      <c r="Z4" s="145">
         <v>2014</v>
       </c>
-      <c r="AA4" s="141"/>
-      <c r="AB4" s="141"/>
-      <c r="AC4" s="141"/>
-      <c r="AD4" s="141"/>
-      <c r="AE4" s="141"/>
-      <c r="AF4" s="141"/>
-      <c r="AG4" s="141"/>
-      <c r="AH4" s="141"/>
-      <c r="AI4" s="141"/>
-      <c r="AJ4" s="141"/>
-      <c r="AK4" s="141"/>
-      <c r="AL4" s="144">
+      <c r="AA4" s="142"/>
+      <c r="AB4" s="142"/>
+      <c r="AC4" s="142"/>
+      <c r="AD4" s="142"/>
+      <c r="AE4" s="142"/>
+      <c r="AF4" s="142"/>
+      <c r="AG4" s="142"/>
+      <c r="AH4" s="142"/>
+      <c r="AI4" s="142"/>
+      <c r="AJ4" s="142"/>
+      <c r="AK4" s="142"/>
+      <c r="AL4" s="145">
         <v>2015</v>
       </c>
-      <c r="AM4" s="141"/>
-      <c r="AN4" s="141"/>
-      <c r="AO4" s="141"/>
-      <c r="AP4" s="141"/>
-      <c r="AQ4" s="141"/>
-      <c r="AR4" s="141"/>
-      <c r="AS4" s="141"/>
-      <c r="AT4" s="141"/>
-      <c r="AU4" s="141"/>
-      <c r="AV4" s="141"/>
-      <c r="AW4" s="141"/>
-      <c r="AX4" s="144">
+      <c r="AM4" s="142"/>
+      <c r="AN4" s="142"/>
+      <c r="AO4" s="142"/>
+      <c r="AP4" s="142"/>
+      <c r="AQ4" s="142"/>
+      <c r="AR4" s="142"/>
+      <c r="AS4" s="142"/>
+      <c r="AT4" s="142"/>
+      <c r="AU4" s="142"/>
+      <c r="AV4" s="142"/>
+      <c r="AW4" s="142"/>
+      <c r="AX4" s="145">
         <v>2016</v>
       </c>
-      <c r="AY4" s="141"/>
-      <c r="AZ4" s="141"/>
-      <c r="BA4" s="141"/>
-      <c r="BB4" s="141"/>
-      <c r="BC4" s="141"/>
-      <c r="BD4" s="141"/>
-      <c r="BE4" s="141"/>
-      <c r="BF4" s="141"/>
-      <c r="BG4" s="141"/>
-      <c r="BH4" s="141"/>
-      <c r="BI4" s="141"/>
-      <c r="BJ4" s="144">
+      <c r="AY4" s="142"/>
+      <c r="AZ4" s="142"/>
+      <c r="BA4" s="142"/>
+      <c r="BB4" s="142"/>
+      <c r="BC4" s="142"/>
+      <c r="BD4" s="142"/>
+      <c r="BE4" s="142"/>
+      <c r="BF4" s="142"/>
+      <c r="BG4" s="142"/>
+      <c r="BH4" s="142"/>
+      <c r="BI4" s="142"/>
+      <c r="BJ4" s="145">
         <v>2017</v>
       </c>
-      <c r="BK4" s="141"/>
-      <c r="BL4" s="141"/>
-      <c r="BM4" s="141"/>
-      <c r="BN4" s="141"/>
-      <c r="BO4" s="141"/>
-      <c r="BP4" s="141"/>
-      <c r="BQ4" s="141"/>
-      <c r="BR4" s="141"/>
-      <c r="BS4" s="141"/>
-      <c r="BT4" s="141"/>
-      <c r="BU4" s="141"/>
-      <c r="BV4" s="157">
+      <c r="BK4" s="142"/>
+      <c r="BL4" s="142"/>
+      <c r="BM4" s="142"/>
+      <c r="BN4" s="142"/>
+      <c r="BO4" s="142"/>
+      <c r="BP4" s="142"/>
+      <c r="BQ4" s="142"/>
+      <c r="BR4" s="142"/>
+      <c r="BS4" s="142"/>
+      <c r="BT4" s="142"/>
+      <c r="BU4" s="142"/>
+      <c r="BV4" s="158">
         <v>2018</v>
       </c>
-      <c r="BW4" s="158"/>
-      <c r="BX4" s="158"/>
-      <c r="BY4" s="158"/>
-      <c r="BZ4" s="158"/>
-      <c r="CA4" s="158"/>
-      <c r="CB4" s="158"/>
-      <c r="CC4" s="158"/>
-      <c r="CD4" s="158"/>
-      <c r="CE4" s="158"/>
-      <c r="CF4" s="158"/>
-      <c r="CG4" s="158"/>
-      <c r="CH4" s="157">
+      <c r="BW4" s="159"/>
+      <c r="BX4" s="159"/>
+      <c r="BY4" s="159"/>
+      <c r="BZ4" s="159"/>
+      <c r="CA4" s="159"/>
+      <c r="CB4" s="159"/>
+      <c r="CC4" s="159"/>
+      <c r="CD4" s="159"/>
+      <c r="CE4" s="159"/>
+      <c r="CF4" s="159"/>
+      <c r="CG4" s="159"/>
+      <c r="CH4" s="158">
         <v>2019</v>
       </c>
-      <c r="CI4" s="158"/>
-      <c r="CJ4" s="158"/>
-      <c r="CK4" s="158"/>
-      <c r="CL4" s="158"/>
-      <c r="CM4" s="158"/>
-      <c r="CN4" s="158"/>
-      <c r="CO4" s="158"/>
-      <c r="CP4" s="158"/>
-      <c r="CQ4" s="158"/>
-      <c r="CR4" s="158"/>
-      <c r="CS4" s="158"/>
-      <c r="CT4" s="157">
+      <c r="CI4" s="159"/>
+      <c r="CJ4" s="159"/>
+      <c r="CK4" s="159"/>
+      <c r="CL4" s="159"/>
+      <c r="CM4" s="159"/>
+      <c r="CN4" s="159"/>
+      <c r="CO4" s="159"/>
+      <c r="CP4" s="159"/>
+      <c r="CQ4" s="159"/>
+      <c r="CR4" s="159"/>
+      <c r="CS4" s="159"/>
+      <c r="CT4" s="158">
         <v>2020</v>
       </c>
-      <c r="CU4" s="158"/>
-      <c r="CV4" s="158"/>
-      <c r="CW4" s="158"/>
-      <c r="CX4" s="158"/>
-      <c r="CY4" s="158"/>
-      <c r="CZ4" s="158"/>
-      <c r="DA4" s="158"/>
-      <c r="DB4" s="158"/>
-      <c r="DC4" s="158"/>
-      <c r="DD4" s="158"/>
-      <c r="DE4" s="158"/>
-      <c r="DF4" s="144">
+      <c r="CU4" s="159"/>
+      <c r="CV4" s="159"/>
+      <c r="CW4" s="159"/>
+      <c r="CX4" s="159"/>
+      <c r="CY4" s="159"/>
+      <c r="CZ4" s="159"/>
+      <c r="DA4" s="159"/>
+      <c r="DB4" s="159"/>
+      <c r="DC4" s="159"/>
+      <c r="DD4" s="159"/>
+      <c r="DE4" s="159"/>
+      <c r="DF4" s="145">
         <v>2021</v>
       </c>
-      <c r="DG4" s="141"/>
-      <c r="DH4" s="141"/>
-      <c r="DI4" s="141"/>
-      <c r="DJ4" s="141"/>
-      <c r="DK4" s="141"/>
-      <c r="DL4" s="141"/>
-      <c r="DM4" s="141"/>
-      <c r="DN4" s="145"/>
-      <c r="DO4" s="141"/>
-      <c r="DP4" s="141"/>
-      <c r="DQ4" s="141"/>
-      <c r="DR4" s="142" t="s">
+      <c r="DG4" s="142"/>
+      <c r="DH4" s="142"/>
+      <c r="DI4" s="142"/>
+      <c r="DJ4" s="142"/>
+      <c r="DK4" s="142"/>
+      <c r="DL4" s="142"/>
+      <c r="DM4" s="142"/>
+      <c r="DN4" s="146"/>
+      <c r="DO4" s="142"/>
+      <c r="DP4" s="142"/>
+      <c r="DQ4" s="142"/>
+      <c r="DR4" s="143" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:122" ht="18" customHeight="1">
-      <c r="A5" s="156"/>
+      <c r="A5" s="157"/>
       <c r="B5" s="50" t="s">
         <v>2</v>
       </c>
@@ -26618,10 +26744,10 @@
         <v>2</v>
       </c>
       <c r="DG5" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="DH5" s="50" t="s">
         <v>104</v>
-      </c>
-      <c r="DH5" s="50" t="s">
-        <v>4</v>
       </c>
       <c r="DI5" s="50" t="s">
         <v>5</v>
@@ -26650,7 +26776,7 @@
       <c r="DQ5" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="DR5" s="147"/>
+      <c r="DR5" s="148"/>
     </row>
     <row r="6" spans="1:122" ht="18" customHeight="1">
       <c r="A6" s="52" t="s">
@@ -27032,9 +27158,11 @@
         <v>-49.694912787702769</v>
       </c>
       <c r="DG6" s="54">
-        <v>-47.731547785237893</v>
-      </c>
-      <c r="DH6" s="54"/>
+        <v>-48.345578130533163</v>
+      </c>
+      <c r="DH6" s="54">
+        <v>-41.960709450335706</v>
+      </c>
       <c r="DI6" s="54"/>
       <c r="DJ6" s="54"/>
       <c r="DK6" s="54"/>
@@ -27428,9 +27556,11 @@
         <v>-31.661250057469786</v>
       </c>
       <c r="DG7" s="58">
-        <v>-31.368149760625812</v>
-      </c>
-      <c r="DH7" s="58"/>
+        <v>-32.285228502690288</v>
+      </c>
+      <c r="DH7" s="58">
+        <v>-30.113980399620871</v>
+      </c>
       <c r="DI7" s="58"/>
       <c r="DJ7" s="58"/>
       <c r="DK7" s="58"/>
@@ -27824,9 +27954,11 @@
         <v>13.397994616371605</v>
       </c>
       <c r="DG8" s="54">
-        <v>9.13885575054789</v>
-      </c>
-      <c r="DH8" s="54"/>
+        <v>8.9157991540436541</v>
+      </c>
+      <c r="DH8" s="54">
+        <v>1.7221872770999909</v>
+      </c>
       <c r="DI8" s="54"/>
       <c r="DJ8" s="54"/>
       <c r="DK8" s="54"/>
@@ -28220,9 +28352,11 @@
         <v>-14.017601221166458</v>
       </c>
       <c r="DG9" s="58">
-        <v>-12.616191859044065</v>
-      </c>
-      <c r="DH9" s="58"/>
+        <v>-13.799510877411251</v>
+      </c>
+      <c r="DH9" s="58">
+        <v>-4.2086998722064664</v>
+      </c>
       <c r="DI9" s="58"/>
       <c r="DJ9" s="58"/>
       <c r="DK9" s="58"/>
@@ -28616,9 +28750,11 @@
         <v>-38.445203684997978</v>
       </c>
       <c r="DG10" s="54">
-        <v>-33.349186916490922</v>
-      </c>
-      <c r="DH10" s="54"/>
+        <v>-39.779247288790017</v>
+      </c>
+      <c r="DH10" s="54">
+        <v>-42.701748476556858</v>
+      </c>
       <c r="DI10" s="54"/>
       <c r="DJ10" s="54"/>
       <c r="DK10" s="54"/>
@@ -29012,9 +29148,11 @@
         <v>-14.351479134794957</v>
       </c>
       <c r="DG11" s="58">
-        <v>-21.4282791666935</v>
-      </c>
-      <c r="DH11" s="58"/>
+        <v>-26.545642150695883</v>
+      </c>
+      <c r="DH11" s="58">
+        <v>38.329728090413226</v>
+      </c>
       <c r="DI11" s="58"/>
       <c r="DJ11" s="58"/>
       <c r="DK11" s="58"/>
@@ -29408,9 +29546,11 @@
         <v>-3.8699901830057399</v>
       </c>
       <c r="DG12" s="54">
-        <v>-6.1220739400956603</v>
-      </c>
-      <c r="DH12" s="54"/>
+        <v>-7.6803788305527405</v>
+      </c>
+      <c r="DH12" s="54">
+        <v>-1.254600861166395</v>
+      </c>
       <c r="DI12" s="54"/>
       <c r="DJ12" s="54"/>
       <c r="DK12" s="54"/>
@@ -29804,9 +29944,11 @@
         <v>-6.3741418758748694</v>
       </c>
       <c r="DG13" s="58">
-        <v>-5.3120246639137321</v>
-      </c>
-      <c r="DH13" s="58"/>
+        <v>-8.4497218874897726</v>
+      </c>
+      <c r="DH13" s="58">
+        <v>61.384842637617339</v>
+      </c>
       <c r="DI13" s="58"/>
       <c r="DJ13" s="58"/>
       <c r="DK13" s="58"/>
@@ -30200,9 +30342,11 @@
         <v>-33.211840462163423</v>
       </c>
       <c r="DG14" s="54">
-        <v>-33.027216082370572</v>
-      </c>
-      <c r="DH14" s="54"/>
+        <v>-33.749490782020615</v>
+      </c>
+      <c r="DH14" s="54">
+        <v>-20.90565161655384</v>
+      </c>
       <c r="DI14" s="54"/>
       <c r="DJ14" s="54"/>
       <c r="DK14" s="54"/>
@@ -30596,9 +30740,11 @@
         <v>-16.351743828103054</v>
       </c>
       <c r="DG15" s="62">
-        <v>-16.504557664251422</v>
-      </c>
-      <c r="DH15" s="115"/>
+        <v>-18.133187367329214</v>
+      </c>
+      <c r="DH15" s="62">
+        <v>-17.083498111989883</v>
+      </c>
       <c r="DI15" s="115"/>
       <c r="DJ15" s="115"/>
       <c r="DK15" s="115"/>
@@ -30738,7 +30884,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BJ6" sqref="BJ6:DG15"/>
+      <selection pane="topRight" activeCell="BJ6" sqref="BJ6:DH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -30750,8 +30896,8 @@
     <col min="77" max="77" width="5.6328125" bestFit="1" customWidth="1"/>
     <col min="80" max="91" width="9.08984375" customWidth="1"/>
     <col min="92" max="92" width="9.81640625" customWidth="1"/>
-    <col min="93" max="111" width="9.08984375" customWidth="1"/>
-    <col min="112" max="121" width="9.08984375" hidden="1" customWidth="1"/>
+    <col min="93" max="112" width="9.08984375" customWidth="1"/>
+    <col min="113" max="121" width="9.08984375" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="28.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -30917,155 +31063,155 @@
       <c r="BX3" s="3"/>
     </row>
     <row r="4" spans="1:122" ht="18" customHeight="1">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="M4" s="141"/>
-      <c r="N4" s="144">
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="145">
         <v>2013</v>
       </c>
-      <c r="O4" s="141"/>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="141"/>
-      <c r="R4" s="141"/>
-      <c r="S4" s="141"/>
-      <c r="T4" s="141"/>
-      <c r="U4" s="141"/>
-      <c r="V4" s="141"/>
-      <c r="W4" s="141"/>
-      <c r="X4" s="141"/>
-      <c r="Y4" s="141"/>
-      <c r="Z4" s="144">
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
+      <c r="Q4" s="142"/>
+      <c r="R4" s="142"/>
+      <c r="S4" s="142"/>
+      <c r="T4" s="142"/>
+      <c r="U4" s="142"/>
+      <c r="V4" s="142"/>
+      <c r="W4" s="142"/>
+      <c r="X4" s="142"/>
+      <c r="Y4" s="142"/>
+      <c r="Z4" s="145">
         <v>2014</v>
       </c>
-      <c r="AA4" s="141"/>
-      <c r="AB4" s="141"/>
-      <c r="AC4" s="141"/>
-      <c r="AD4" s="141"/>
-      <c r="AE4" s="141"/>
-      <c r="AF4" s="141"/>
-      <c r="AG4" s="141"/>
-      <c r="AH4" s="141"/>
-      <c r="AI4" s="141"/>
-      <c r="AJ4" s="141"/>
-      <c r="AK4" s="141"/>
-      <c r="AL4" s="144">
+      <c r="AA4" s="142"/>
+      <c r="AB4" s="142"/>
+      <c r="AC4" s="142"/>
+      <c r="AD4" s="142"/>
+      <c r="AE4" s="142"/>
+      <c r="AF4" s="142"/>
+      <c r="AG4" s="142"/>
+      <c r="AH4" s="142"/>
+      <c r="AI4" s="142"/>
+      <c r="AJ4" s="142"/>
+      <c r="AK4" s="142"/>
+      <c r="AL4" s="145">
         <v>2015</v>
       </c>
-      <c r="AM4" s="141"/>
-      <c r="AN4" s="141"/>
-      <c r="AO4" s="141"/>
-      <c r="AP4" s="141"/>
-      <c r="AQ4" s="141"/>
-      <c r="AR4" s="141"/>
-      <c r="AS4" s="141"/>
-      <c r="AT4" s="141"/>
-      <c r="AU4" s="141"/>
-      <c r="AV4" s="141"/>
-      <c r="AW4" s="141"/>
-      <c r="AX4" s="144">
+      <c r="AM4" s="142"/>
+      <c r="AN4" s="142"/>
+      <c r="AO4" s="142"/>
+      <c r="AP4" s="142"/>
+      <c r="AQ4" s="142"/>
+      <c r="AR4" s="142"/>
+      <c r="AS4" s="142"/>
+      <c r="AT4" s="142"/>
+      <c r="AU4" s="142"/>
+      <c r="AV4" s="142"/>
+      <c r="AW4" s="142"/>
+      <c r="AX4" s="145">
         <v>2016</v>
       </c>
-      <c r="AY4" s="141"/>
-      <c r="AZ4" s="141"/>
-      <c r="BA4" s="141"/>
-      <c r="BB4" s="141"/>
-      <c r="BC4" s="141"/>
-      <c r="BD4" s="141"/>
-      <c r="BE4" s="141"/>
-      <c r="BF4" s="141"/>
-      <c r="BG4" s="141"/>
-      <c r="BH4" s="141"/>
-      <c r="BI4" s="141"/>
-      <c r="BJ4" s="144">
+      <c r="AY4" s="142"/>
+      <c r="AZ4" s="142"/>
+      <c r="BA4" s="142"/>
+      <c r="BB4" s="142"/>
+      <c r="BC4" s="142"/>
+      <c r="BD4" s="142"/>
+      <c r="BE4" s="142"/>
+      <c r="BF4" s="142"/>
+      <c r="BG4" s="142"/>
+      <c r="BH4" s="142"/>
+      <c r="BI4" s="142"/>
+      <c r="BJ4" s="145">
         <v>2017</v>
       </c>
-      <c r="BK4" s="141"/>
-      <c r="BL4" s="141"/>
-      <c r="BM4" s="141"/>
-      <c r="BN4" s="141"/>
-      <c r="BO4" s="141"/>
-      <c r="BP4" s="141"/>
-      <c r="BQ4" s="141"/>
-      <c r="BR4" s="141"/>
-      <c r="BS4" s="141"/>
-      <c r="BT4" s="141"/>
-      <c r="BU4" s="141"/>
-      <c r="BV4" s="157">
+      <c r="BK4" s="142"/>
+      <c r="BL4" s="142"/>
+      <c r="BM4" s="142"/>
+      <c r="BN4" s="142"/>
+      <c r="BO4" s="142"/>
+      <c r="BP4" s="142"/>
+      <c r="BQ4" s="142"/>
+      <c r="BR4" s="142"/>
+      <c r="BS4" s="142"/>
+      <c r="BT4" s="142"/>
+      <c r="BU4" s="142"/>
+      <c r="BV4" s="158">
         <v>2018</v>
       </c>
-      <c r="BW4" s="158"/>
-      <c r="BX4" s="158"/>
-      <c r="BY4" s="158"/>
-      <c r="BZ4" s="158"/>
-      <c r="CA4" s="158"/>
-      <c r="CB4" s="158"/>
-      <c r="CC4" s="158"/>
-      <c r="CD4" s="158"/>
-      <c r="CE4" s="158"/>
-      <c r="CF4" s="158"/>
-      <c r="CG4" s="158"/>
-      <c r="CH4" s="157">
+      <c r="BW4" s="159"/>
+      <c r="BX4" s="159"/>
+      <c r="BY4" s="159"/>
+      <c r="BZ4" s="159"/>
+      <c r="CA4" s="159"/>
+      <c r="CB4" s="159"/>
+      <c r="CC4" s="159"/>
+      <c r="CD4" s="159"/>
+      <c r="CE4" s="159"/>
+      <c r="CF4" s="159"/>
+      <c r="CG4" s="159"/>
+      <c r="CH4" s="158">
         <v>2019</v>
       </c>
-      <c r="CI4" s="158"/>
-      <c r="CJ4" s="158"/>
-      <c r="CK4" s="158"/>
-      <c r="CL4" s="158"/>
-      <c r="CM4" s="158"/>
-      <c r="CN4" s="158"/>
-      <c r="CO4" s="158"/>
-      <c r="CP4" s="158"/>
-      <c r="CQ4" s="158"/>
-      <c r="CR4" s="158"/>
-      <c r="CS4" s="158"/>
-      <c r="CT4" s="157">
+      <c r="CI4" s="159"/>
+      <c r="CJ4" s="159"/>
+      <c r="CK4" s="159"/>
+      <c r="CL4" s="159"/>
+      <c r="CM4" s="159"/>
+      <c r="CN4" s="159"/>
+      <c r="CO4" s="159"/>
+      <c r="CP4" s="159"/>
+      <c r="CQ4" s="159"/>
+      <c r="CR4" s="159"/>
+      <c r="CS4" s="159"/>
+      <c r="CT4" s="158">
         <v>2020</v>
       </c>
-      <c r="CU4" s="158"/>
-      <c r="CV4" s="158"/>
-      <c r="CW4" s="158"/>
-      <c r="CX4" s="158"/>
-      <c r="CY4" s="158"/>
-      <c r="CZ4" s="158"/>
-      <c r="DA4" s="158"/>
-      <c r="DB4" s="158"/>
-      <c r="DC4" s="158"/>
-      <c r="DD4" s="158"/>
-      <c r="DE4" s="158"/>
-      <c r="DF4" s="144">
+      <c r="CU4" s="159"/>
+      <c r="CV4" s="159"/>
+      <c r="CW4" s="159"/>
+      <c r="CX4" s="159"/>
+      <c r="CY4" s="159"/>
+      <c r="CZ4" s="159"/>
+      <c r="DA4" s="159"/>
+      <c r="DB4" s="159"/>
+      <c r="DC4" s="159"/>
+      <c r="DD4" s="159"/>
+      <c r="DE4" s="159"/>
+      <c r="DF4" s="145">
         <v>2021</v>
       </c>
-      <c r="DG4" s="141"/>
-      <c r="DH4" s="141"/>
-      <c r="DI4" s="141"/>
-      <c r="DJ4" s="141"/>
-      <c r="DK4" s="141"/>
-      <c r="DL4" s="141"/>
-      <c r="DM4" s="141"/>
-      <c r="DN4" s="145"/>
-      <c r="DO4" s="141"/>
-      <c r="DP4" s="141"/>
-      <c r="DQ4" s="141"/>
-      <c r="DR4" s="142" t="s">
+      <c r="DG4" s="142"/>
+      <c r="DH4" s="142"/>
+      <c r="DI4" s="142"/>
+      <c r="DJ4" s="142"/>
+      <c r="DK4" s="142"/>
+      <c r="DL4" s="142"/>
+      <c r="DM4" s="142"/>
+      <c r="DN4" s="146"/>
+      <c r="DO4" s="142"/>
+      <c r="DP4" s="142"/>
+      <c r="DQ4" s="142"/>
+      <c r="DR4" s="143" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:122" ht="18" customHeight="1">
-      <c r="A5" s="156"/>
+      <c r="A5" s="157"/>
       <c r="B5" s="50" t="s">
         <v>2</v>
       </c>
@@ -31394,10 +31540,10 @@
         <v>2</v>
       </c>
       <c r="DG5" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="DH5" s="50" t="s">
         <v>104</v>
-      </c>
-      <c r="DH5" s="50" t="s">
-        <v>4</v>
       </c>
       <c r="DI5" s="50" t="s">
         <v>5</v>
@@ -31426,7 +31572,7 @@
       <c r="DQ5" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="DR5" s="147"/>
+      <c r="DR5" s="148"/>
     </row>
     <row r="6" spans="1:122" ht="18" customHeight="1">
       <c r="A6" s="52" t="s">
@@ -31819,9 +31965,11 @@
         <v>-6.7006129058711537</v>
       </c>
       <c r="DG6" s="54">
-        <v>3.7549649026469893</v>
-      </c>
-      <c r="DH6" s="54"/>
+        <v>2.5360901469243089</v>
+      </c>
+      <c r="DH6" s="54">
+        <v>2.0828119343269123</v>
+      </c>
       <c r="DI6" s="54"/>
       <c r="DJ6" s="54"/>
       <c r="DK6" s="54"/>
@@ -32226,9 +32374,11 @@
         <v>-4.7782036970322679</v>
       </c>
       <c r="DG7" s="58">
-        <v>-0.87729973424353602</v>
-      </c>
-      <c r="DH7" s="58"/>
+        <v>-2.2018060815546079</v>
+      </c>
+      <c r="DH7" s="58">
+        <v>-0.37818296974234045</v>
+      </c>
       <c r="DI7" s="58"/>
       <c r="DJ7" s="58"/>
       <c r="DK7" s="58"/>
@@ -32633,9 +32783,11 @@
         <v>-1.7832621354211682</v>
       </c>
       <c r="DG8" s="54">
-        <v>-1.4945170769215963</v>
-      </c>
-      <c r="DH8" s="54"/>
+        <v>-1.6958413221386195</v>
+      </c>
+      <c r="DH8" s="54">
+        <v>3.9888698493383288</v>
+      </c>
       <c r="DI8" s="54"/>
       <c r="DJ8" s="54"/>
       <c r="DK8" s="54"/>
@@ -33040,9 +33192,11 @@
         <v>-2.4975197134448024</v>
       </c>
       <c r="DG9" s="58">
-        <v>2.9159306128860862E-3</v>
-      </c>
-      <c r="DH9" s="58"/>
+        <v>-1.3512863504548704</v>
+      </c>
+      <c r="DH9" s="58">
+        <v>0.92856209452133953</v>
+      </c>
       <c r="DI9" s="58"/>
       <c r="DJ9" s="58"/>
       <c r="DK9" s="58"/>
@@ -33447,9 +33601,11 @@
         <v>-11.578660166028385</v>
       </c>
       <c r="DG10" s="54">
-        <v>1.916627183048476</v>
-      </c>
-      <c r="DH10" s="54"/>
+        <v>-7.9156619580759582</v>
+      </c>
+      <c r="DH10" s="54">
+        <v>5.2369888767626236</v>
+      </c>
       <c r="DI10" s="54"/>
       <c r="DJ10" s="54"/>
       <c r="DK10" s="54"/>
@@ -33854,9 +34010,11 @@
         <v>-3.2192949869595822</v>
       </c>
       <c r="DG11" s="58">
-        <v>-5.9699476645866412</v>
-      </c>
-      <c r="DH11" s="58"/>
+        <v>-12.094109183537071</v>
+      </c>
+      <c r="DH11" s="58">
+        <v>13.467272146888433</v>
+      </c>
       <c r="DI11" s="58"/>
       <c r="DJ11" s="58"/>
       <c r="DK11" s="58"/>
@@ -34261,9 +34419,11 @@
         <v>-5.670571604738285</v>
       </c>
       <c r="DG12" s="54">
-        <v>-5.3507725321609598</v>
-      </c>
-      <c r="DH12" s="54"/>
+        <v>-6.9218804616970573</v>
+      </c>
+      <c r="DH12" s="54">
+        <v>8.5142633837942583</v>
+      </c>
       <c r="DI12" s="54"/>
       <c r="DJ12" s="54"/>
       <c r="DK12" s="54"/>
@@ -34668,9 +34828,11 @@
         <v>-29.812996281268596</v>
       </c>
       <c r="DG13" s="58">
-        <v>1.1986710421918048</v>
-      </c>
-      <c r="DH13" s="58"/>
+        <v>-2.1547726029133401</v>
+      </c>
+      <c r="DH13" s="58">
+        <v>-4.0275761662924339</v>
+      </c>
       <c r="DI13" s="58"/>
       <c r="DJ13" s="58"/>
       <c r="DK13" s="58"/>
@@ -35075,9 +35237,11 @@
         <v>-2.9185219189069187</v>
       </c>
       <c r="DG14" s="54">
-        <v>-0.95496495950176552</v>
-      </c>
-      <c r="DH14" s="54"/>
+        <v>-2.0231260654174008</v>
+      </c>
+      <c r="DH14" s="54">
+        <v>1.111025520607285</v>
+      </c>
       <c r="DI14" s="54"/>
       <c r="DJ14" s="54"/>
       <c r="DK14" s="54"/>
@@ -35482,9 +35646,11 @@
         <v>-4.2571274409940827</v>
       </c>
       <c r="DG15" s="62">
-        <v>-0.72459170655693583</v>
-      </c>
-      <c r="DH15" s="115"/>
+        <v>-2.6610193031881977</v>
+      </c>
+      <c r="DH15" s="62">
+        <v>2.9395063091537423</v>
+      </c>
       <c r="DI15" s="115"/>
       <c r="DJ15" s="115"/>
       <c r="DK15" s="115"/>
@@ -35619,13 +35785,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AL20"/>
+  <dimension ref="A2:AP20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="W6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6:AK15"/>
+      <selection pane="bottomRight" activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -35638,11 +35804,12 @@
     <col min="26" max="26" width="8" style="48" customWidth="1"/>
     <col min="27" max="27" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6.81640625" customWidth="1"/>
-    <col min="29" max="37" width="7.54296875" customWidth="1"/>
-    <col min="38" max="38" width="27.6328125" customWidth="1"/>
+    <col min="29" max="38" width="7.54296875" customWidth="1"/>
+    <col min="39" max="41" width="7.54296875" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="27.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:38" s="16" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:42" s="16" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>93</v>
       </c>
@@ -35671,11 +35838,11 @@
       <c r="X2" s="11"/>
       <c r="Y2" s="11"/>
       <c r="Z2" s="49"/>
-      <c r="AL2" s="19" t="s">
+      <c r="AP2" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15" customHeight="1" thickBot="1">
+    <row r="3" spans="1:42" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="6"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -35703,70 +35870,76 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="49"/>
     </row>
-    <row r="4" spans="1:38" ht="18" customHeight="1">
-      <c r="A4" s="155" t="s">
+    <row r="4" spans="1:42" ht="18" customHeight="1">
+      <c r="A4" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="150">
+      <c r="B4" s="151">
         <v>2012</v>
       </c>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="148">
+      <c r="C4" s="149"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="149">
         <v>2013</v>
       </c>
-      <c r="G4" s="148"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="149"/>
-      <c r="J4" s="148">
+      <c r="G4" s="149"/>
+      <c r="H4" s="149"/>
+      <c r="I4" s="150"/>
+      <c r="J4" s="149">
         <v>2014</v>
       </c>
-      <c r="K4" s="148"/>
-      <c r="L4" s="148"/>
-      <c r="M4" s="149"/>
-      <c r="N4" s="148">
+      <c r="K4" s="149"/>
+      <c r="L4" s="149"/>
+      <c r="M4" s="150"/>
+      <c r="N4" s="149">
         <v>2015</v>
       </c>
-      <c r="O4" s="148"/>
-      <c r="P4" s="148"/>
-      <c r="Q4" s="149"/>
-      <c r="R4" s="148">
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="150"/>
+      <c r="R4" s="149">
         <v>2016</v>
       </c>
-      <c r="S4" s="148"/>
-      <c r="T4" s="148"/>
-      <c r="U4" s="149"/>
-      <c r="V4" s="148">
+      <c r="S4" s="149"/>
+      <c r="T4" s="149"/>
+      <c r="U4" s="150"/>
+      <c r="V4" s="149">
         <v>2017</v>
       </c>
-      <c r="W4" s="148"/>
-      <c r="X4" s="148"/>
-      <c r="Y4" s="149"/>
-      <c r="Z4" s="148">
+      <c r="W4" s="149"/>
+      <c r="X4" s="149"/>
+      <c r="Y4" s="150"/>
+      <c r="Z4" s="149">
         <v>2018</v>
       </c>
-      <c r="AA4" s="148"/>
-      <c r="AB4" s="148"/>
-      <c r="AC4" s="149"/>
-      <c r="AD4" s="148">
+      <c r="AA4" s="149"/>
+      <c r="AB4" s="149"/>
+      <c r="AC4" s="150"/>
+      <c r="AD4" s="149">
         <v>2019</v>
       </c>
-      <c r="AE4" s="148"/>
-      <c r="AF4" s="148"/>
-      <c r="AG4" s="149"/>
-      <c r="AH4" s="148">
+      <c r="AE4" s="149"/>
+      <c r="AF4" s="149"/>
+      <c r="AG4" s="150"/>
+      <c r="AH4" s="149">
         <v>2020</v>
       </c>
-      <c r="AI4" s="148"/>
-      <c r="AJ4" s="148"/>
-      <c r="AK4" s="149"/>
-      <c r="AL4" s="142" t="s">
+      <c r="AI4" s="149"/>
+      <c r="AJ4" s="149"/>
+      <c r="AK4" s="150"/>
+      <c r="AL4" s="149">
+        <v>2021</v>
+      </c>
+      <c r="AM4" s="149"/>
+      <c r="AN4" s="149"/>
+      <c r="AO4" s="150"/>
+      <c r="AP4" s="143" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="18" customHeight="1">
-      <c r="A5" s="156"/>
+    <row r="5" spans="1:42" ht="18" customHeight="1">
+      <c r="A5" s="157"/>
       <c r="B5" s="81" t="s">
         <v>32</v>
       </c>
@@ -35875,9 +36048,21 @@
       <c r="AK5" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="147"/>
+      <c r="AL5" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM5" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN5" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO5" s="121" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP5" s="148"/>
     </row>
-    <row r="6" spans="1:38" ht="18" customHeight="1">
+    <row r="6" spans="1:42" ht="18" customHeight="1">
       <c r="A6" s="69" t="s">
         <v>39</v>
       </c>
@@ -35986,14 +36171,20 @@
       <c r="AJ6" s="117">
         <v>-45.155620862648256</v>
       </c>
-      <c r="AK6" s="117">
+      <c r="AK6" s="85">
         <v>-48.069855259853959</v>
       </c>
-      <c r="AL6" s="66" t="s">
+      <c r="AL6" s="117">
+        <v>-46.667066789523879</v>
+      </c>
+      <c r="AM6" s="117"/>
+      <c r="AN6" s="117"/>
+      <c r="AO6" s="117"/>
+      <c r="AP6" s="66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="18" customHeight="1">
+    <row r="7" spans="1:42" ht="18" customHeight="1">
       <c r="A7" s="70" t="s">
         <v>40</v>
       </c>
@@ -36102,14 +36293,20 @@
       <c r="AJ7" s="118">
         <v>-16.751899893435223</v>
       </c>
-      <c r="AK7" s="118">
+      <c r="AK7" s="86">
         <v>-29.616462483595388</v>
       </c>
-      <c r="AL7" s="67" t="s">
+      <c r="AL7" s="118">
+        <v>-31.353486319926983</v>
+      </c>
+      <c r="AM7" s="118"/>
+      <c r="AN7" s="118"/>
+      <c r="AO7" s="118"/>
+      <c r="AP7" s="67" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="18" customHeight="1">
+    <row r="8" spans="1:42" ht="18" customHeight="1">
       <c r="A8" s="69" t="s">
         <v>41</v>
       </c>
@@ -36218,14 +36415,20 @@
       <c r="AJ8" s="117">
         <v>4.7802587082615604</v>
       </c>
-      <c r="AK8" s="117">
+      <c r="AK8" s="85">
         <v>6.7873537194635505</v>
       </c>
-      <c r="AL8" s="66" t="s">
+      <c r="AL8" s="117">
+        <v>8.0119936825050839</v>
+      </c>
+      <c r="AM8" s="117"/>
+      <c r="AN8" s="117"/>
+      <c r="AO8" s="117"/>
+      <c r="AP8" s="66" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="18" customHeight="1">
+    <row r="9" spans="1:42" ht="18" customHeight="1">
       <c r="A9" s="70" t="s">
         <v>42</v>
       </c>
@@ -36334,14 +36537,20 @@
       <c r="AJ9" s="118">
         <v>-18.930803518680332</v>
       </c>
-      <c r="AK9" s="118">
+      <c r="AK9" s="86">
         <v>-15.071972247040263</v>
       </c>
-      <c r="AL9" s="67" t="s">
+      <c r="AL9" s="118">
+        <v>-10.675270656928056</v>
+      </c>
+      <c r="AM9" s="118"/>
+      <c r="AN9" s="118"/>
+      <c r="AO9" s="118"/>
+      <c r="AP9" s="67" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="18" customHeight="1">
+    <row r="10" spans="1:42" ht="18" customHeight="1">
       <c r="A10" s="69" t="s">
         <v>43</v>
       </c>
@@ -36450,14 +36659,20 @@
       <c r="AJ10" s="117">
         <v>-11.385451927993321</v>
       </c>
-      <c r="AK10" s="117">
+      <c r="AK10" s="85">
         <v>-30.624677598770148</v>
       </c>
-      <c r="AL10" s="66" t="s">
+      <c r="AL10" s="117">
+        <v>-40.308733150114954</v>
+      </c>
+      <c r="AM10" s="117"/>
+      <c r="AN10" s="117"/>
+      <c r="AO10" s="117"/>
+      <c r="AP10" s="66" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="18" customHeight="1">
+    <row r="11" spans="1:42" ht="18" customHeight="1">
       <c r="A11" s="70" t="s">
         <v>44</v>
       </c>
@@ -36566,14 +36781,20 @@
       <c r="AJ11" s="118">
         <v>-37.182211334960236</v>
       </c>
-      <c r="AK11" s="118">
+      <c r="AK11" s="86">
         <v>-12.838591369390857</v>
       </c>
-      <c r="AL11" s="67" t="s">
+      <c r="AL11" s="118">
+        <v>-0.85579773169253082</v>
+      </c>
+      <c r="AM11" s="118"/>
+      <c r="AN11" s="118"/>
+      <c r="AO11" s="118"/>
+      <c r="AP11" s="67" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="18" customHeight="1">
+    <row r="12" spans="1:42" ht="18" customHeight="1">
       <c r="A12" s="52" t="s">
         <v>103</v>
       </c>
@@ -36682,14 +36903,20 @@
       <c r="AJ12" s="117">
         <v>3.1305947185759067</v>
       </c>
-      <c r="AK12" s="117">
+      <c r="AK12" s="85">
         <v>-1.2578602397289436</v>
       </c>
-      <c r="AL12" s="66" t="s">
+      <c r="AL12" s="117">
+        <v>-4.2683232915749647</v>
+      </c>
+      <c r="AM12" s="117"/>
+      <c r="AN12" s="117"/>
+      <c r="AO12" s="117"/>
+      <c r="AP12" s="66" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="18" customHeight="1">
+    <row r="13" spans="1:42" ht="18" customHeight="1">
       <c r="A13" s="70" t="s">
         <v>46</v>
       </c>
@@ -36798,14 +37025,20 @@
       <c r="AJ13" s="118">
         <v>9.8673906107254172</v>
       </c>
-      <c r="AK13" s="118">
+      <c r="AK13" s="86">
         <v>10.436072931990632</v>
       </c>
-      <c r="AL13" s="67" t="s">
+      <c r="AL13" s="118">
+        <v>15.520326291417566</v>
+      </c>
+      <c r="AM13" s="118"/>
+      <c r="AN13" s="118"/>
+      <c r="AO13" s="118"/>
+      <c r="AP13" s="67" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="18" customHeight="1">
+    <row r="14" spans="1:42" ht="18" customHeight="1">
       <c r="A14" s="69" t="s">
         <v>47</v>
       </c>
@@ -36914,14 +37147,20 @@
       <c r="AJ14" s="117">
         <v>-31.814601509990087</v>
       </c>
-      <c r="AK14" s="117">
+      <c r="AK14" s="85">
         <v>-31.991273333936761</v>
       </c>
-      <c r="AL14" s="66" t="s">
+      <c r="AL14" s="117">
+        <v>-29.288994286912626</v>
+      </c>
+      <c r="AM14" s="117"/>
+      <c r="AN14" s="117"/>
+      <c r="AO14" s="117"/>
+      <c r="AP14" s="66" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="18" customHeight="1" thickBot="1">
+    <row r="15" spans="1:42" ht="18" customHeight="1" thickBot="1">
       <c r="A15" s="60" t="s">
         <v>22</v>
       </c>
@@ -37030,14 +37269,20 @@
       <c r="AJ15" s="119">
         <v>-10.06733208233031</v>
       </c>
-      <c r="AK15" s="119">
+      <c r="AK15" s="122">
         <v>-16.792045380275134</v>
       </c>
-      <c r="AL15" s="68" t="s">
+      <c r="AL15" s="119">
+        <v>-17.189476435807389</v>
+      </c>
+      <c r="AM15" s="119"/>
+      <c r="AN15" s="119"/>
+      <c r="AO15" s="119"/>
+      <c r="AP15" s="68" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:38" s="32" customFormat="1" ht="16.5" customHeight="1">
+    <row r="16" spans="1:42" s="32" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="31" t="s">
         <v>68</v>
       </c>
@@ -37066,11 +37311,11 @@
       <c r="X16" s="24"/>
       <c r="Y16" s="24"/>
       <c r="Z16" s="24"/>
-      <c r="AL16" s="45" t="s">
+      <c r="AP16" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:38" s="20" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="17" spans="1:42" s="20" customFormat="1" ht="15" hidden="1" customHeight="1">
       <c r="A17" s="124" t="s">
         <v>87</v>
       </c>
@@ -37110,43 +37355,47 @@
       <c r="AI17" s="125"/>
       <c r="AJ17" s="125"/>
       <c r="AK17" s="125"/>
-      <c r="AL17" s="127" t="s">
+      <c r="AL17" s="125"/>
+      <c r="AM17" s="125"/>
+      <c r="AN17" s="125"/>
+      <c r="AO17" s="125"/>
+      <c r="AP17" s="127" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:38" s="42" customFormat="1" ht="15" customHeight="1">
+    <row r="18" spans="1:42" s="42" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="31" t="s">
         <v>91</v>
       </c>
       <c r="W18" s="43"/>
       <c r="Z18" s="128"/>
-      <c r="AL18" s="45" t="s">
+      <c r="AP18" s="45" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:38" s="20" customFormat="1" ht="15" customHeight="1">
+    <row r="19" spans="1:42" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="22" t="s">
         <v>78</v>
       </c>
       <c r="Z19" s="129"/>
-      <c r="AL19" s="33" t="s">
+      <c r="AP19" s="33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:38" s="130" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="20" spans="1:42" s="130" customFormat="1" ht="15" hidden="1" customHeight="1">
       <c r="A20" s="22" t="s">
         <v>102</v>
       </c>
       <c r="Z20" s="131"/>
-      <c r="AL20" s="33" t="s">
+      <c r="AP20" s="33" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="AL4:AL5"/>
+    <mergeCell ref="AP4:AP5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="R4:U4"/>
@@ -37155,6 +37404,7 @@
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="AD4:AG4"/>
     <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="AL4:AO4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -37163,11 +37413,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:DG17"/>
+  <dimension ref="A2:DH17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CU8" sqref="CU8"/>
+      <selection pane="topRight" activeCell="DC14" sqref="DC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -37177,11 +37427,11 @@
     <col min="62" max="62" width="8.90625" collapsed="1"/>
     <col min="80" max="82" width="9.08984375" customWidth="1"/>
     <col min="83" max="83" width="9.36328125" customWidth="1"/>
-    <col min="84" max="110" width="9.08984375" customWidth="1"/>
-    <col min="111" max="111" width="36.453125" customWidth="1"/>
+    <col min="84" max="111" width="9.08984375" customWidth="1"/>
+    <col min="112" max="112" width="36.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:111" s="16" customFormat="1" ht="14.4" customHeight="1">
+    <row r="2" spans="1:112" s="16" customFormat="1" ht="14.4" customHeight="1">
       <c r="A2" s="39" t="s">
         <v>72</v>
       </c>
@@ -37294,11 +37544,12 @@
       <c r="DD2" s="3"/>
       <c r="DE2" s="3"/>
       <c r="DF2" s="3"/>
-      <c r="DG2" s="40" t="s">
+      <c r="DG2" s="3"/>
+      <c r="DH2" s="40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:111" ht="14.4" customHeight="1" thickBot="1">
+    <row r="3" spans="1:112" ht="14.4" customHeight="1" thickBot="1">
       <c r="A3" s="14"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -37409,123 +37660,124 @@
       <c r="DD3" s="8"/>
       <c r="DE3" s="8"/>
       <c r="DF3" s="8"/>
+      <c r="DG3" s="8"/>
     </row>
-    <row r="4" spans="1:111" ht="18" customHeight="1">
-      <c r="A4" s="163" t="s">
+    <row r="4" spans="1:112" ht="18" customHeight="1">
+      <c r="A4" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="161">
+      <c r="B4" s="162">
         <v>2012</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="161"/>
-      <c r="I4" s="161"/>
-      <c r="J4" s="161"/>
-      <c r="K4" s="161"/>
-      <c r="L4" s="161"/>
-      <c r="M4" s="162"/>
-      <c r="N4" s="161">
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="162"/>
+      <c r="G4" s="162"/>
+      <c r="H4" s="162"/>
+      <c r="I4" s="162"/>
+      <c r="J4" s="162"/>
+      <c r="K4" s="162"/>
+      <c r="L4" s="162"/>
+      <c r="M4" s="163"/>
+      <c r="N4" s="162">
         <v>2013</v>
       </c>
-      <c r="O4" s="161"/>
-      <c r="P4" s="161"/>
-      <c r="Q4" s="161"/>
-      <c r="R4" s="161"/>
-      <c r="S4" s="161"/>
-      <c r="T4" s="161"/>
-      <c r="U4" s="161"/>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
-      <c r="Z4" s="161">
+      <c r="O4" s="162"/>
+      <c r="P4" s="162"/>
+      <c r="Q4" s="162"/>
+      <c r="R4" s="162"/>
+      <c r="S4" s="162"/>
+      <c r="T4" s="162"/>
+      <c r="U4" s="162"/>
+      <c r="V4" s="162"/>
+      <c r="W4" s="162"/>
+      <c r="X4" s="162"/>
+      <c r="Y4" s="163"/>
+      <c r="Z4" s="162">
         <v>2014</v>
       </c>
-      <c r="AA4" s="161"/>
-      <c r="AB4" s="161"/>
-      <c r="AC4" s="161"/>
-      <c r="AD4" s="161"/>
-      <c r="AE4" s="161"/>
-      <c r="AF4" s="161"/>
-      <c r="AG4" s="161"/>
-      <c r="AH4" s="161"/>
-      <c r="AI4" s="161"/>
-      <c r="AJ4" s="161"/>
-      <c r="AK4" s="162"/>
-      <c r="AL4" s="161">
+      <c r="AA4" s="162"/>
+      <c r="AB4" s="162"/>
+      <c r="AC4" s="162"/>
+      <c r="AD4" s="162"/>
+      <c r="AE4" s="162"/>
+      <c r="AF4" s="162"/>
+      <c r="AG4" s="162"/>
+      <c r="AH4" s="162"/>
+      <c r="AI4" s="162"/>
+      <c r="AJ4" s="162"/>
+      <c r="AK4" s="163"/>
+      <c r="AL4" s="162">
         <v>2015</v>
       </c>
-      <c r="AM4" s="161"/>
-      <c r="AN4" s="161"/>
-      <c r="AO4" s="161"/>
-      <c r="AP4" s="161"/>
-      <c r="AQ4" s="161"/>
-      <c r="AR4" s="161"/>
-      <c r="AS4" s="161"/>
-      <c r="AT4" s="161"/>
-      <c r="AU4" s="161"/>
-      <c r="AV4" s="161"/>
-      <c r="AW4" s="162"/>
-      <c r="AX4" s="161">
+      <c r="AM4" s="162"/>
+      <c r="AN4" s="162"/>
+      <c r="AO4" s="162"/>
+      <c r="AP4" s="162"/>
+      <c r="AQ4" s="162"/>
+      <c r="AR4" s="162"/>
+      <c r="AS4" s="162"/>
+      <c r="AT4" s="162"/>
+      <c r="AU4" s="162"/>
+      <c r="AV4" s="162"/>
+      <c r="AW4" s="163"/>
+      <c r="AX4" s="162">
         <v>2016</v>
       </c>
-      <c r="AY4" s="161"/>
-      <c r="AZ4" s="161"/>
-      <c r="BA4" s="161"/>
-      <c r="BB4" s="161"/>
-      <c r="BC4" s="161"/>
-      <c r="BD4" s="161"/>
-      <c r="BE4" s="161"/>
-      <c r="BF4" s="161"/>
-      <c r="BG4" s="161"/>
-      <c r="BH4" s="161"/>
-      <c r="BI4" s="162"/>
-      <c r="BJ4" s="161">
+      <c r="AY4" s="162"/>
+      <c r="AZ4" s="162"/>
+      <c r="BA4" s="162"/>
+      <c r="BB4" s="162"/>
+      <c r="BC4" s="162"/>
+      <c r="BD4" s="162"/>
+      <c r="BE4" s="162"/>
+      <c r="BF4" s="162"/>
+      <c r="BG4" s="162"/>
+      <c r="BH4" s="162"/>
+      <c r="BI4" s="163"/>
+      <c r="BJ4" s="162">
         <v>2017</v>
       </c>
-      <c r="BK4" s="161"/>
-      <c r="BL4" s="161"/>
-      <c r="BM4" s="161"/>
-      <c r="BN4" s="161"/>
-      <c r="BO4" s="161"/>
-      <c r="BP4" s="161"/>
-      <c r="BQ4" s="161"/>
-      <c r="BR4" s="161"/>
-      <c r="BS4" s="161"/>
-      <c r="BT4" s="161"/>
-      <c r="BU4" s="162"/>
-      <c r="BV4" s="165">
+      <c r="BK4" s="162"/>
+      <c r="BL4" s="162"/>
+      <c r="BM4" s="162"/>
+      <c r="BN4" s="162"/>
+      <c r="BO4" s="162"/>
+      <c r="BP4" s="162"/>
+      <c r="BQ4" s="162"/>
+      <c r="BR4" s="162"/>
+      <c r="BS4" s="162"/>
+      <c r="BT4" s="162"/>
+      <c r="BU4" s="163"/>
+      <c r="BV4" s="166">
         <v>2018</v>
       </c>
-      <c r="BW4" s="166"/>
-      <c r="BX4" s="166"/>
-      <c r="BY4" s="166"/>
-      <c r="BZ4" s="166"/>
-      <c r="CA4" s="166"/>
-      <c r="CB4" s="166"/>
-      <c r="CC4" s="166"/>
-      <c r="CD4" s="166"/>
-      <c r="CE4" s="166"/>
-      <c r="CF4" s="166"/>
-      <c r="CG4" s="167"/>
-      <c r="CH4" s="165">
+      <c r="BW4" s="167"/>
+      <c r="BX4" s="167"/>
+      <c r="BY4" s="167"/>
+      <c r="BZ4" s="167"/>
+      <c r="CA4" s="167"/>
+      <c r="CB4" s="167"/>
+      <c r="CC4" s="167"/>
+      <c r="CD4" s="167"/>
+      <c r="CE4" s="167"/>
+      <c r="CF4" s="167"/>
+      <c r="CG4" s="168"/>
+      <c r="CH4" s="166">
         <v>2019</v>
       </c>
-      <c r="CI4" s="166"/>
-      <c r="CJ4" s="166"/>
-      <c r="CK4" s="166"/>
-      <c r="CL4" s="166"/>
-      <c r="CM4" s="166"/>
-      <c r="CN4" s="166"/>
-      <c r="CO4" s="166"/>
-      <c r="CP4" s="166"/>
-      <c r="CQ4" s="166"/>
-      <c r="CR4" s="166"/>
-      <c r="CS4" s="167"/>
+      <c r="CI4" s="167"/>
+      <c r="CJ4" s="167"/>
+      <c r="CK4" s="167"/>
+      <c r="CL4" s="167"/>
+      <c r="CM4" s="167"/>
+      <c r="CN4" s="167"/>
+      <c r="CO4" s="167"/>
+      <c r="CP4" s="167"/>
+      <c r="CQ4" s="167"/>
+      <c r="CR4" s="167"/>
+      <c r="CS4" s="168"/>
       <c r="CT4" s="134">
         <v>2020</v>
       </c>
@@ -37540,15 +37792,16 @@
       <c r="DC4" s="135"/>
       <c r="DD4" s="135"/>
       <c r="DE4" s="136"/>
-      <c r="DF4" s="137">
+      <c r="DF4" s="169">
         <v>2021</v>
       </c>
-      <c r="DG4" s="159" t="s">
+      <c r="DG4" s="170"/>
+      <c r="DH4" s="160" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:111" ht="18" customHeight="1">
-      <c r="A5" s="164"/>
+    <row r="5" spans="1:112" ht="18" customHeight="1">
+      <c r="A5" s="165"/>
       <c r="B5" s="110" t="s">
         <v>2</v>
       </c>
@@ -37876,9 +38129,12 @@
       <c r="DF5" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="DG5" s="160"/>
+      <c r="DG5" s="137" t="s">
+        <v>3</v>
+      </c>
+      <c r="DH5" s="161"/>
     </row>
-    <row r="6" spans="1:111" ht="18" customHeight="1" thickBot="1">
+    <row r="6" spans="1:112" ht="18" customHeight="1" thickBot="1">
       <c r="A6" s="104"/>
       <c r="B6" s="87"/>
       <c r="C6" s="88"/>
@@ -37989,9 +38245,10 @@
       <c r="DD6" s="120"/>
       <c r="DE6" s="120"/>
       <c r="DF6" s="120"/>
-      <c r="DG6" s="90"/>
+      <c r="DG6" s="120"/>
+      <c r="DH6" s="90"/>
     </row>
-    <row r="7" spans="1:111" ht="18" customHeight="1">
+    <row r="7" spans="1:112" ht="18" customHeight="1">
       <c r="A7" s="96" t="s">
         <v>48</v>
       </c>
@@ -38104,11 +38361,12 @@
       <c r="DD7" s="97"/>
       <c r="DE7" s="97"/>
       <c r="DF7" s="97"/>
-      <c r="DG7" s="99" t="s">
+      <c r="DG7" s="138"/>
+      <c r="DH7" s="99" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:111" ht="18" customHeight="1">
+    <row r="8" spans="1:112" ht="18" customHeight="1">
       <c r="A8" s="105" t="s">
         <v>49</v>
       </c>
@@ -38516,11 +38774,14 @@
       <c r="DF8" s="92">
         <v>156.90489455207259</v>
       </c>
-      <c r="DG8" s="94" t="s">
+      <c r="DG8" s="92">
+        <v>156.41926634670708</v>
+      </c>
+      <c r="DH8" s="94" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:111" ht="18" customHeight="1">
+    <row r="9" spans="1:112" ht="18" customHeight="1">
       <c r="A9" s="105" t="s">
         <v>50</v>
       </c>
@@ -38928,11 +39189,14 @@
       <c r="DF9" s="92">
         <v>153.47175725957467</v>
       </c>
-      <c r="DG9" s="94" t="s">
+      <c r="DG9" s="92">
+        <v>141.70240653397957</v>
+      </c>
+      <c r="DH9" s="94" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:111" ht="18" customHeight="1" thickBot="1">
+    <row r="10" spans="1:112" ht="18" customHeight="1" thickBot="1">
       <c r="A10" s="106"/>
       <c r="B10" s="91"/>
       <c r="C10" s="92"/>
@@ -39043,9 +39307,10 @@
       <c r="DD10" s="92"/>
       <c r="DE10" s="92"/>
       <c r="DF10" s="92"/>
-      <c r="DG10" s="95"/>
+      <c r="DG10" s="92"/>
+      <c r="DH10" s="95"/>
     </row>
-    <row r="11" spans="1:111" ht="18" customHeight="1">
+    <row r="11" spans="1:112" ht="18" customHeight="1">
       <c r="A11" s="96" t="s">
         <v>51</v>
       </c>
@@ -39158,11 +39423,12 @@
       <c r="DD11" s="97"/>
       <c r="DE11" s="97"/>
       <c r="DF11" s="97"/>
-      <c r="DG11" s="99" t="s">
+      <c r="DG11" s="138"/>
+      <c r="DH11" s="99" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:111" ht="18" customHeight="1">
+    <row r="12" spans="1:112" ht="18" customHeight="1">
       <c r="A12" s="105" t="s">
         <v>49</v>
       </c>
@@ -39570,11 +39836,14 @@
       <c r="DF12" s="92">
         <v>150.3875968992248</v>
       </c>
-      <c r="DG12" s="94" t="s">
+      <c r="DG12" s="92">
+        <v>150.51813471502589</v>
+      </c>
+      <c r="DH12" s="94" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:111" ht="18" customHeight="1">
+    <row r="13" spans="1:112" ht="18" customHeight="1">
       <c r="A13" s="105" t="s">
         <v>50</v>
       </c>
@@ -39982,11 +40251,14 @@
       <c r="DF13" s="92">
         <v>154.07503234152651</v>
       </c>
-      <c r="DG13" s="94" t="s">
+      <c r="DG13" s="92">
+        <v>151.36186770428014</v>
+      </c>
+      <c r="DH13" s="94" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:111" ht="18" customHeight="1" thickBot="1">
+    <row r="14" spans="1:112" ht="18" customHeight="1" thickBot="1">
       <c r="A14" s="107"/>
       <c r="B14" s="101"/>
       <c r="C14" s="102"/>
@@ -40097,9 +40369,10 @@
       <c r="DD14" s="102"/>
       <c r="DE14" s="102"/>
       <c r="DF14" s="102"/>
-      <c r="DG14" s="112"/>
+      <c r="DG14" s="102"/>
+      <c r="DH14" s="112"/>
     </row>
-    <row r="15" spans="1:111" s="41" customFormat="1" ht="16.5" customHeight="1">
+    <row r="15" spans="1:112" s="41" customFormat="1" ht="16.5" customHeight="1">
       <c r="A15" s="31"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -40210,9 +40483,10 @@
       <c r="DD15" s="26"/>
       <c r="DE15" s="26"/>
       <c r="DF15" s="26"/>
-      <c r="DG15" s="31"/>
+      <c r="DG15" s="26"/>
+      <c r="DH15" s="31"/>
     </row>
-    <row r="16" spans="1:111" s="44" customFormat="1" ht="16.5" customHeight="1">
+    <row r="16" spans="1:112" s="44" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="31"/>
       <c r="B16" s="42"/>
       <c r="C16" s="42"/>
@@ -40322,15 +40596,16 @@
       <c r="DD16" s="29"/>
       <c r="DE16" s="29"/>
       <c r="DF16" s="29"/>
-      <c r="DG16" s="31"/>
+      <c r="DG16" s="29"/>
+      <c r="DH16" s="31"/>
     </row>
-    <row r="17" spans="1:111" s="44" customFormat="1" ht="14.4" customHeight="1">
+    <row r="17" spans="1:112" s="44" customFormat="1" ht="14.4" customHeight="1">
       <c r="A17" s="31"/>
-      <c r="DG17" s="31"/>
+      <c r="DH17" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="DG4:DG5"/>
+  <mergeCells count="11">
+    <mergeCell ref="DH4:DH5"/>
     <mergeCell ref="BJ4:BU4"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:M4"/>
@@ -40340,6 +40615,7 @@
     <mergeCell ref="AX4:BI4"/>
     <mergeCell ref="BV4:CG4"/>
     <mergeCell ref="CH4:CS4"/>
+    <mergeCell ref="DF4:DG4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update retail sales index
</commit_message>
<xml_diff>
--- a/data/bi_rsi_raw.xlsx
+++ b/data/bi_rsi_raw.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Safira Widya Putri\Departemen Statistik\SURVEI\SPE\Data Bulanan\2021\04. April 2021\Permintaan Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Safira Widya Putri\Departemen Statistik\SURVEI\SPE\Data Bulanan\2021\05. Mei 2021\Permintaan Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-150" yWindow="420" windowWidth="12000" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Tabel 1" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="107">
   <si>
     <t>DESKRIPSI</t>
   </si>
@@ -550,10 +550,13 @@
     <t>Makassar</t>
   </si>
   <si>
-    <t>Mei*</t>
+    <t>Q2*</t>
   </si>
   <si>
-    <t>Q2*</t>
+    <t>Jun*</t>
+  </si>
+  <si>
+    <t>May</t>
   </si>
 </sst>
 </file>
@@ -2256,8 +2259,8 @@
   <dimension ref="A2:DR17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DI6" sqref="DI6:DJ14"/>
+      <pane xSplit="1" topLeftCell="DF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DJ6" sqref="DJ6:DK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -2265,8 +2268,8 @@
     <col min="1" max="1" width="44.453125" customWidth="1"/>
     <col min="2" max="62" width="9.453125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="63" max="63" width="9.453125" customWidth="1" collapsed="1"/>
-    <col min="64" max="114" width="9.453125" customWidth="1"/>
-    <col min="115" max="121" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="64" max="115" width="9.453125" customWidth="1"/>
+    <col min="116" max="121" width="9.453125" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="43.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3008,10 +3011,10 @@
         <v>5</v>
       </c>
       <c r="DJ5" s="50" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="DK5" s="50" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="DL5" s="50" t="s">
         <v>8</v>
@@ -3374,9 +3377,11 @@
         <v>122.75266418772952</v>
       </c>
       <c r="DJ6" s="54">
-        <v>124.34700620016339</v>
-      </c>
-      <c r="DK6" s="54"/>
+        <v>123.00786324906538</v>
+      </c>
+      <c r="DK6" s="54">
+        <v>122.72321368548067</v>
+      </c>
       <c r="DL6" s="54"/>
       <c r="DM6" s="54"/>
       <c r="DN6" s="54"/>
@@ -3728,9 +3733,11 @@
         <v>287.27408730848816</v>
       </c>
       <c r="DJ7" s="58">
-        <v>291.15143528385954</v>
-      </c>
-      <c r="DK7" s="58"/>
+        <v>296.44932678890103</v>
+      </c>
+      <c r="DK7" s="58">
+        <v>254.54691450089766</v>
+      </c>
       <c r="DL7" s="58"/>
       <c r="DM7" s="58"/>
       <c r="DN7" s="58"/>
@@ -4082,9 +4089,11 @@
         <v>74.372314103109971</v>
       </c>
       <c r="DJ8" s="54">
-        <v>77.350303735790348</v>
-      </c>
-      <c r="DK8" s="54"/>
+        <v>74.519999244248851</v>
+      </c>
+      <c r="DK8" s="54">
+        <v>82.716637588587801</v>
+      </c>
       <c r="DL8" s="54"/>
       <c r="DM8" s="54"/>
       <c r="DN8" s="54"/>
@@ -4436,9 +4445,11 @@
         <v>188.082082537167</v>
       </c>
       <c r="DJ9" s="58">
-        <v>192.16012755882156</v>
-      </c>
-      <c r="DK9" s="58"/>
+        <v>189.98772414070874</v>
+      </c>
+      <c r="DK9" s="58">
+        <v>189.21237138926</v>
+      </c>
       <c r="DL9" s="58"/>
       <c r="DM9" s="58"/>
       <c r="DN9" s="58"/>
@@ -4790,9 +4801,11 @@
         <v>127.48722043463879</v>
       </c>
       <c r="DJ10" s="54">
-        <v>128.31422223491035</v>
-      </c>
-      <c r="DK10" s="54"/>
+        <v>132.23515670406076</v>
+      </c>
+      <c r="DK10" s="54">
+        <v>131.89658856207924</v>
+      </c>
       <c r="DL10" s="54"/>
       <c r="DM10" s="54"/>
       <c r="DN10" s="54"/>
@@ -5144,9 +5157,11 @@
         <v>58.166502312193558</v>
       </c>
       <c r="DJ11" s="58">
-        <v>58.818112105652617</v>
-      </c>
-      <c r="DK11" s="58"/>
+        <v>59.368258233301994</v>
+      </c>
+      <c r="DK11" s="58">
+        <v>61.759154925226269</v>
+      </c>
       <c r="DL11" s="58"/>
       <c r="DM11" s="58"/>
       <c r="DN11" s="58"/>
@@ -5498,9 +5513,11 @@
         <v>100.05533309058457</v>
       </c>
       <c r="DJ12" s="54">
-        <v>105.81048842423075</v>
-      </c>
-      <c r="DK12" s="54"/>
+        <v>112.1039854549816</v>
+      </c>
+      <c r="DK12" s="54">
+        <v>99.15707022013288</v>
+      </c>
       <c r="DL12" s="54"/>
       <c r="DM12" s="54"/>
       <c r="DN12" s="54"/>
@@ -5852,9 +5869,11 @@
         <v>80.323663032440379</v>
       </c>
       <c r="DJ13" s="58">
-        <v>86.018236468051342</v>
-      </c>
-      <c r="DK13" s="58"/>
+        <v>95.120021133512722</v>
+      </c>
+      <c r="DK13" s="58">
+        <v>87.18809530768489</v>
+      </c>
       <c r="DL13" s="58"/>
       <c r="DM13" s="58"/>
       <c r="DN13" s="58"/>
@@ -6206,9 +6225,11 @@
         <v>220.40696796060118</v>
       </c>
       <c r="DJ14" s="115">
-        <v>223.896867022549</v>
-      </c>
-      <c r="DK14" s="115"/>
+        <v>227.51262899059833</v>
+      </c>
+      <c r="DK14" s="115">
+        <v>202.32517096888276</v>
+      </c>
       <c r="DL14" s="115"/>
       <c r="DM14" s="115"/>
       <c r="DN14" s="115"/>
@@ -6509,8 +6530,8 @@
   <dimension ref="A2:DT17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DI6" sqref="DI6:DJ14"/>
+      <pane xSplit="1" topLeftCell="DF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DJ6" sqref="DJ6:DK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -6525,8 +6546,8 @@
     <col min="79" max="79" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="80" max="100" width="7" customWidth="1"/>
     <col min="101" max="101" width="7.1796875" customWidth="1"/>
-    <col min="102" max="114" width="7" customWidth="1"/>
-    <col min="115" max="121" width="7" hidden="1" customWidth="1"/>
+    <col min="102" max="115" width="7" customWidth="1"/>
+    <col min="116" max="121" width="7" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7178,10 +7199,10 @@
         <v>5</v>
       </c>
       <c r="DJ5" s="50" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="DK5" s="50" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="DL5" s="50" t="s">
         <v>8</v>
@@ -7643,9 +7664,11 @@
         <v>8.1330764070528296</v>
       </c>
       <c r="DJ6" s="54">
-        <v>41.094437792530016</v>
-      </c>
-      <c r="DK6" s="54"/>
+        <v>39.574935010896063</v>
+      </c>
+      <c r="DK6" s="54">
+        <v>24.388326142552973</v>
+      </c>
       <c r="DL6" s="54"/>
       <c r="DM6" s="54"/>
       <c r="DN6" s="54"/>
@@ -8096,9 +8119,11 @@
         <v>26.675041839313462</v>
       </c>
       <c r="DJ7" s="58">
-        <v>19.81833042508714</v>
-      </c>
-      <c r="DK7" s="58"/>
+        <v>21.998585914085279</v>
+      </c>
+      <c r="DK7" s="58">
+        <v>9.3510686829026959</v>
+      </c>
       <c r="DL7" s="58"/>
       <c r="DM7" s="58"/>
       <c r="DN7" s="58"/>
@@ -8549,9 +8574,11 @@
         <v>37.3070601313362</v>
       </c>
       <c r="DJ8" s="54">
-        <v>59.352236733492724</v>
-      </c>
-      <c r="DK8" s="54"/>
+        <v>53.521421215242839</v>
+      </c>
+      <c r="DK8" s="54">
+        <v>48.848910417496548</v>
+      </c>
       <c r="DL8" s="54"/>
       <c r="DM8" s="54"/>
       <c r="DN8" s="54"/>
@@ -9002,9 +9029,11 @@
         <v>-31.07923969901417</v>
       </c>
       <c r="DJ9" s="58">
-        <v>-27.738911184848348</v>
-      </c>
-      <c r="DK9" s="58"/>
+        <v>-28.555835269635587</v>
+      </c>
+      <c r="DK9" s="58">
+        <v>-31.722894165248839</v>
+      </c>
       <c r="DL9" s="58"/>
       <c r="DM9" s="58"/>
       <c r="DN9" s="58"/>
@@ -9455,9 +9484,11 @@
         <v>-10.818461252582834</v>
       </c>
       <c r="DJ10" s="54">
-        <v>-10.178411029683964</v>
-      </c>
-      <c r="DK10" s="54"/>
+        <v>-7.433706988827038</v>
+      </c>
+      <c r="DK10" s="54">
+        <v>-5.1650931078721101</v>
+      </c>
       <c r="DL10" s="54"/>
       <c r="DM10" s="54"/>
       <c r="DN10" s="54"/>
@@ -9908,9 +9939,11 @@
         <v>-7.786816489663984</v>
       </c>
       <c r="DJ11" s="58">
-        <v>7.4310593506199174</v>
-      </c>
-      <c r="DK11" s="58"/>
+        <v>8.4358991724906129</v>
+      </c>
+      <c r="DK11" s="58">
+        <v>-1.2094792627652562</v>
+      </c>
       <c r="DL11" s="58"/>
       <c r="DM11" s="58"/>
       <c r="DN11" s="58"/>
@@ -10361,9 +10394,11 @@
         <v>48.15396535251206</v>
       </c>
       <c r="DJ12" s="54">
-        <v>35.077779302136982</v>
-      </c>
-      <c r="DK12" s="54"/>
+        <v>43.112064141178898</v>
+      </c>
+      <c r="DK12" s="54">
+        <v>38.216012035699151</v>
+      </c>
       <c r="DL12" s="54"/>
       <c r="DM12" s="54"/>
       <c r="DN12" s="54"/>
@@ -10814,9 +10849,11 @@
         <v>55.152572904700527</v>
       </c>
       <c r="DJ13" s="58">
-        <v>37.65389212925372</v>
-      </c>
-      <c r="DK13" s="58"/>
+        <v>52.219362615136824</v>
+      </c>
+      <c r="DK13" s="58">
+        <v>53.814842270060346</v>
+      </c>
       <c r="DL13" s="58"/>
       <c r="DM13" s="58"/>
       <c r="DN13" s="58"/>
@@ -11267,9 +11304,11 @@
         <v>15.599528028887267</v>
       </c>
       <c r="DJ14" s="115">
-        <v>12.909375322064509</v>
-      </c>
-      <c r="DK14" s="115"/>
+        <v>14.73277477626327</v>
+      </c>
+      <c r="DK14" s="115">
+        <v>4.523171016015759</v>
+      </c>
       <c r="DL14" s="115"/>
       <c r="DM14" s="115"/>
       <c r="DN14" s="115"/>
@@ -11570,8 +11609,8 @@
   <dimension ref="A2:DR17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DI6" sqref="DI6:DJ14"/>
+      <pane xSplit="1" topLeftCell="DF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DJ6" sqref="DJ6:DK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -11583,8 +11622,8 @@
     <col min="63" max="73" width="9.453125" customWidth="1"/>
     <col min="74" max="76" width="8.54296875" customWidth="1"/>
     <col min="77" max="77" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="80" max="114" width="9.1796875" customWidth="1"/>
-    <col min="115" max="121" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="80" max="115" width="9.1796875" customWidth="1"/>
+    <col min="116" max="121" width="9.1796875" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="43.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12235,10 +12274,10 @@
         <v>5</v>
       </c>
       <c r="DJ5" s="50" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="DK5" s="50" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="DL5" s="50" t="s">
         <v>8</v>
@@ -12711,9 +12750,11 @@
         <v>4.0571706491525195</v>
       </c>
       <c r="DJ6" s="54">
-        <v>1.2988247733634495</v>
-      </c>
-      <c r="DK6" s="54"/>
+        <v>0.20789696339753583</v>
+      </c>
+      <c r="DK6" s="54">
+        <v>-0.23140761579473201</v>
+      </c>
       <c r="DL6" s="54"/>
       <c r="DM6" s="54"/>
       <c r="DN6" s="54"/>
@@ -13175,9 +13216,11 @@
         <v>22.39116539654551</v>
       </c>
       <c r="DJ7" s="58">
-        <v>1.3497033483593324</v>
-      </c>
-      <c r="DK7" s="58"/>
+        <v>3.1938973564852313</v>
+      </c>
+      <c r="DK7" s="58">
+        <v>-14.134763853871634</v>
+      </c>
       <c r="DL7" s="58"/>
       <c r="DM7" s="58"/>
       <c r="DN7" s="58"/>
@@ -13639,9 +13682,11 @@
         <v>3.5344025909885612</v>
       </c>
       <c r="DJ8" s="54">
-        <v>4.0041642761736274</v>
-      </c>
-      <c r="DK8" s="54"/>
+        <v>0.19857542812791174</v>
+      </c>
+      <c r="DK8" s="54">
+        <v>10.999246413668651</v>
+      </c>
       <c r="DL8" s="54"/>
       <c r="DM8" s="54"/>
       <c r="DN8" s="54"/>
@@ -14103,9 +14148,11 @@
         <v>1.1981259063705174</v>
       </c>
       <c r="DJ9" s="58">
-        <v>2.1682262162578292</v>
-      </c>
-      <c r="DK9" s="58"/>
+        <v>1.0131967797438524</v>
+      </c>
+      <c r="DK9" s="58">
+        <v>-0.40810676318986383</v>
+      </c>
       <c r="DL9" s="58"/>
       <c r="DM9" s="58"/>
       <c r="DN9" s="58"/>
@@ -14567,9 +14614,11 @@
         <v>0.32335795859548266</v>
       </c>
       <c r="DJ10" s="54">
-        <v>0.6486938827688693</v>
-      </c>
-      <c r="DK10" s="54"/>
+        <v>3.7242448719447818</v>
+      </c>
+      <c r="DK10" s="54">
+        <v>-0.25603489300445315</v>
+      </c>
       <c r="DL10" s="54"/>
       <c r="DM10" s="54"/>
       <c r="DN10" s="54"/>
@@ -15031,9 +15080,11 @@
         <v>0.11583486008144295</v>
       </c>
       <c r="DJ11" s="58">
-        <v>1.1202492286053412</v>
-      </c>
-      <c r="DK11" s="58"/>
+        <v>2.0660618626478833</v>
+      </c>
+      <c r="DK11" s="58">
+        <v>4.0272306499689936</v>
+      </c>
       <c r="DL11" s="58"/>
       <c r="DM11" s="58"/>
       <c r="DN11" s="58"/>
@@ -15495,9 +15546,11 @@
         <v>16.820546615756516</v>
       </c>
       <c r="DJ12" s="54">
-        <v>5.7519725894428664</v>
-      </c>
-      <c r="DK12" s="54"/>
+        <v>12.041989159627153</v>
+      </c>
+      <c r="DK12" s="54">
+        <v>-11.549023152301663</v>
+      </c>
       <c r="DL12" s="54"/>
       <c r="DM12" s="54"/>
       <c r="DN12" s="54"/>
@@ -15959,9 +16012,11 @@
         <v>14.871070251709796</v>
       </c>
       <c r="DJ13" s="58">
-        <v>7.0895340434251386</v>
-      </c>
-      <c r="DK13" s="58"/>
+        <v>18.420920489017689</v>
+      </c>
+      <c r="DK13" s="58">
+        <v>-8.338860453672936</v>
+      </c>
       <c r="DL13" s="58"/>
       <c r="DM13" s="58"/>
       <c r="DN13" s="58"/>
@@ -16423,9 +16478,11 @@
         <v>17.316482614877906</v>
       </c>
       <c r="DJ14" s="115">
-        <v>1.5833887168992034</v>
-      </c>
-      <c r="DK14" s="115"/>
+        <v>3.2238822101428921</v>
+      </c>
+      <c r="DK14" s="115">
+        <v>-11.070795556916712</v>
+      </c>
       <c r="DL14" s="115"/>
       <c r="DM14" s="115"/>
       <c r="DN14" s="115"/>
@@ -16723,8 +16780,8 @@
   <dimension ref="A2:AP19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL6" sqref="AL6:AM14"/>
+      <pane xSplit="1" topLeftCell="AH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM6" sqref="AM6:AM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -17011,7 +17068,7 @@
         <v>32</v>
       </c>
       <c r="AM5" s="76" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AN5" s="76" t="s">
         <v>34</v>
@@ -17166,7 +17223,7 @@
         <v>-18.775811398717554</v>
       </c>
       <c r="AM6" s="54">
-        <v>24.613757099791421</v>
+        <v>24.032112520167288</v>
       </c>
       <c r="AN6" s="54"/>
       <c r="AO6" s="54"/>
@@ -17319,7 +17376,7 @@
         <v>-8.6037477156486126</v>
       </c>
       <c r="AM7" s="58">
-        <v>23.246686132200303</v>
+        <v>19.341565478767148</v>
       </c>
       <c r="AN7" s="58"/>
       <c r="AO7" s="58"/>
@@ -17472,7 +17529,7 @@
         <v>-10.460964753510892</v>
       </c>
       <c r="AM8" s="54">
-        <v>48.329648432414459</v>
+        <v>46.559130588025198</v>
       </c>
       <c r="AN8" s="54"/>
       <c r="AO8" s="54"/>
@@ -17625,7 +17682,7 @@
         <v>-39.111136095209197</v>
       </c>
       <c r="AM9" s="58">
-        <v>-29.409075441931257</v>
+        <v>-30.452656377966196</v>
       </c>
       <c r="AN9" s="58"/>
       <c r="AO9" s="58"/>
@@ -17778,7 +17835,7 @@
         <v>-25.489371785792486</v>
       </c>
       <c r="AM10" s="54">
-        <v>-10.4984361411334</v>
+        <v>-7.8057537830939943</v>
       </c>
       <c r="AN10" s="54"/>
       <c r="AO10" s="54"/>
@@ -17931,7 +17988,7 @@
         <v>-48.636658808070727</v>
       </c>
       <c r="AM11" s="58">
-        <v>-0.17787856952203329</v>
+        <v>-0.1867988599795424</v>
       </c>
       <c r="AN11" s="58"/>
       <c r="AO11" s="58"/>
@@ -18084,7 +18141,7 @@
         <v>-35.249012895298314</v>
       </c>
       <c r="AM12" s="54">
-        <v>41.615872327324524</v>
+        <v>43.160680509796698</v>
       </c>
       <c r="AN12" s="54"/>
       <c r="AO12" s="54"/>
@@ -18237,7 +18294,7 @@
         <v>-32.817872267746942</v>
       </c>
       <c r="AM13" s="58">
-        <v>46.403232516977127</v>
+        <v>53.728925929965897</v>
       </c>
       <c r="AN13" s="58"/>
       <c r="AO13" s="58"/>
@@ -18390,7 +18447,7 @@
         <v>-16.349383050386969</v>
       </c>
       <c r="AM14" s="123">
-        <v>14.254451675475888</v>
+        <v>11.6184912737221</v>
       </c>
       <c r="AN14" s="123"/>
       <c r="AO14" s="123"/>
@@ -18660,10 +18717,10 @@
   <dimension ref="A2:FD22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="CX6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="DF6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="DI6" sqref="DI6:DJ15"/>
+      <selection pane="bottomRight" activeCell="DJ6" sqref="DJ6:DK15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -18674,8 +18731,8 @@
     <col min="62" max="62" width="9.453125" customWidth="1" collapsed="1"/>
     <col min="63" max="91" width="9.453125" customWidth="1"/>
     <col min="92" max="92" width="10.1796875" customWidth="1"/>
-    <col min="93" max="114" width="9.453125" customWidth="1"/>
-    <col min="115" max="121" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="93" max="115" width="9.453125" customWidth="1"/>
+    <col min="116" max="121" width="9.453125" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="42.1796875" style="34" customWidth="1"/>
     <col min="125" max="125" width="8.54296875" customWidth="1"/>
   </cols>
@@ -19456,10 +19513,10 @@
         <v>5</v>
       </c>
       <c r="DJ5" s="50" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="DK5" s="50" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="DL5" s="50" t="s">
         <v>8</v>
@@ -19822,9 +19879,11 @@
         <v>54.663421147731682</v>
       </c>
       <c r="DJ6" s="54">
-        <v>55.899833633525503</v>
-      </c>
-      <c r="DK6" s="54"/>
+        <v>52.655374068447003</v>
+      </c>
+      <c r="DK6" s="54">
+        <v>55.322129217601663</v>
+      </c>
       <c r="DL6" s="54"/>
       <c r="DM6" s="54"/>
       <c r="DN6" s="54"/>
@@ -20176,9 +20235,11 @@
         <v>166.9232732370275</v>
       </c>
       <c r="DJ7" s="58">
-        <v>172.09528477301012</v>
-      </c>
-      <c r="DK7" s="58"/>
+        <v>174.24439164521729</v>
+      </c>
+      <c r="DK7" s="58">
+        <v>162.94432792093315</v>
+      </c>
       <c r="DL7" s="58"/>
       <c r="DM7" s="58"/>
       <c r="DN7" s="58"/>
@@ -20530,9 +20591,11 @@
         <v>409.63792003607028</v>
       </c>
       <c r="DJ8" s="54">
-        <v>407.85010721496667</v>
-      </c>
-      <c r="DK8" s="54"/>
+        <v>427.53107091828929</v>
+      </c>
+      <c r="DK8" s="54">
+        <v>355.74973566969396</v>
+      </c>
       <c r="DL8" s="54"/>
       <c r="DM8" s="54"/>
       <c r="DN8" s="54"/>
@@ -20884,9 +20947,11 @@
         <v>176.16619411411293</v>
       </c>
       <c r="DJ9" s="58">
-        <v>182.72470384764031</v>
-      </c>
-      <c r="DK9" s="58"/>
+        <v>182.62650960616546</v>
+      </c>
+      <c r="DK9" s="58">
+        <v>168.14633800994011</v>
+      </c>
       <c r="DL9" s="58"/>
       <c r="DM9" s="58"/>
       <c r="DN9" s="58"/>
@@ -21238,9 +21303,11 @@
         <v>166.4502773462398</v>
       </c>
       <c r="DJ10" s="54">
-        <v>170.91576200741119</v>
-      </c>
-      <c r="DK10" s="54"/>
+        <v>157.18751322017545</v>
+      </c>
+      <c r="DK10" s="54">
+        <v>141.48488154375707</v>
+      </c>
       <c r="DL10" s="54"/>
       <c r="DM10" s="54"/>
       <c r="DN10" s="54"/>
@@ -21592,9 +21659,11 @@
         <v>109.4324342846256</v>
       </c>
       <c r="DJ11" s="58">
-        <v>121.81483904759233</v>
-      </c>
-      <c r="DK11" s="58"/>
+        <v>117.87859140236615</v>
+      </c>
+      <c r="DK11" s="58">
+        <v>117.7950406570655</v>
+      </c>
       <c r="DL11" s="58"/>
       <c r="DM11" s="58"/>
       <c r="DN11" s="58"/>
@@ -21946,9 +22015,11 @@
         <v>193.05013683945504</v>
       </c>
       <c r="DJ12" s="54">
-        <v>196.46058583704846</v>
-      </c>
-      <c r="DK12" s="54"/>
+        <v>174.27318023033385</v>
+      </c>
+      <c r="DK12" s="54">
+        <v>177.62864149242515</v>
+      </c>
       <c r="DL12" s="54"/>
       <c r="DM12" s="54"/>
       <c r="DN12" s="54"/>
@@ -22300,9 +22371,11 @@
         <v>186.78634568140376</v>
       </c>
       <c r="DJ13" s="58">
-        <v>196.6331925496213</v>
-      </c>
-      <c r="DK13" s="58"/>
+        <v>197.88645087082253</v>
+      </c>
+      <c r="DK13" s="58">
+        <v>184.81813075774724</v>
+      </c>
       <c r="DL13" s="58"/>
       <c r="DM13" s="58"/>
       <c r="DN13" s="58"/>
@@ -22654,9 +22727,11 @@
         <v>89.883495661715813</v>
       </c>
       <c r="DJ14" s="54">
-        <v>90.31578270989435</v>
-      </c>
-      <c r="DK14" s="54"/>
+        <v>90.937890862301415</v>
+      </c>
+      <c r="DK14" s="54">
+        <v>91.368513318379399</v>
+      </c>
       <c r="DL14" s="54"/>
       <c r="DM14" s="54"/>
       <c r="DN14" s="54"/>
@@ -23008,9 +23083,11 @@
         <v>220.40696796060118</v>
       </c>
       <c r="DJ15" s="115">
-        <v>223.896867022549</v>
-      </c>
-      <c r="DK15" s="115"/>
+        <v>227.51262899059833</v>
+      </c>
+      <c r="DK15" s="115">
+        <v>202.32517096888276</v>
+      </c>
       <c r="DL15" s="115"/>
       <c r="DM15" s="115"/>
       <c r="DN15" s="115"/>
@@ -23511,8 +23588,8 @@
   <dimension ref="A2:DT19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DI6" sqref="DI6:DJ15"/>
+      <pane xSplit="1" topLeftCell="DF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DJ6" sqref="DJ6:DK15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -23523,8 +23600,8 @@
     <col min="74" max="75" width="8.54296875" customWidth="1"/>
     <col min="76" max="76" width="7.54296875" customWidth="1"/>
     <col min="77" max="77" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="114" width="9.1796875" customWidth="1"/>
-    <col min="115" max="121" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="80" max="115" width="9.1796875" customWidth="1"/>
+    <col min="116" max="121" width="9.1796875" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -24176,10 +24253,10 @@
         <v>5</v>
       </c>
       <c r="DJ5" s="50" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="DK5" s="50" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="DL5" s="50" t="s">
         <v>8</v>
@@ -24641,9 +24718,11 @@
         <v>-5.7862285927634538</v>
       </c>
       <c r="DJ6" s="54">
-        <v>-4.7064900687839861</v>
-      </c>
-      <c r="DK6" s="54"/>
+        <v>-10.237382017643226</v>
+      </c>
+      <c r="DK6" s="54">
+        <v>-24.02621881118263</v>
+      </c>
       <c r="DL6" s="54"/>
       <c r="DM6" s="54"/>
       <c r="DN6" s="54"/>
@@ -25094,9 +25173,11 @@
         <v>-23.238881049246586</v>
       </c>
       <c r="DJ7" s="58">
-        <v>-15.90979323564966</v>
-      </c>
-      <c r="DK7" s="58"/>
+        <v>-14.859684038986011</v>
+      </c>
+      <c r="DK7" s="58">
+        <v>-19.794256088045792</v>
+      </c>
       <c r="DL7" s="58"/>
       <c r="DM7" s="58"/>
       <c r="DN7" s="58"/>
@@ -25547,9 +25628,11 @@
         <v>64.055192319271683</v>
       </c>
       <c r="DJ8" s="54">
-        <v>55.354444668177052</v>
-      </c>
-      <c r="DK8" s="54"/>
+        <v>62.851133114681978</v>
+      </c>
+      <c r="DK8" s="54">
+        <v>37.134164265126948</v>
+      </c>
       <c r="DL8" s="54"/>
       <c r="DM8" s="54"/>
       <c r="DN8" s="54"/>
@@ -26000,9 +26083,11 @@
         <v>8.082574469105829</v>
       </c>
       <c r="DJ9" s="58">
-        <v>19.827146140433282</v>
-      </c>
-      <c r="DK9" s="58"/>
+        <v>19.762752353082181</v>
+      </c>
+      <c r="DK9" s="58">
+        <v>9.9337783708805194</v>
+      </c>
       <c r="DL9" s="58"/>
       <c r="DM9" s="58"/>
       <c r="DN9" s="58"/>
@@ -26453,9 +26538,11 @@
         <v>-5.8356296387463864</v>
       </c>
       <c r="DJ10" s="54">
-        <v>-12.400424309683711</v>
-      </c>
-      <c r="DK10" s="54"/>
+        <v>-19.436573314365933</v>
+      </c>
+      <c r="DK10" s="54">
+        <v>-15.470580522785049</v>
+      </c>
       <c r="DL10" s="54"/>
       <c r="DM10" s="54"/>
       <c r="DN10" s="54"/>
@@ -26906,9 +26993,11 @@
         <v>42.776454280692747</v>
       </c>
       <c r="DJ11" s="58">
-        <v>57.781739034443149</v>
-      </c>
-      <c r="DK11" s="58"/>
+        <v>52.683279736792457</v>
+      </c>
+      <c r="DK11" s="58">
+        <v>43.874678438185668</v>
+      </c>
       <c r="DL11" s="58"/>
       <c r="DM11" s="58"/>
       <c r="DN11" s="58"/>
@@ -27359,9 +27448,11 @@
         <v>21.063566434148484</v>
       </c>
       <c r="DJ12" s="54">
-        <v>16.492724977766905</v>
-      </c>
-      <c r="DK12" s="54"/>
+        <v>3.336542386226693</v>
+      </c>
+      <c r="DK12" s="54">
+        <v>5.7579464043494566</v>
+      </c>
       <c r="DL12" s="54"/>
       <c r="DM12" s="54"/>
       <c r="DN12" s="54"/>
@@ -27812,9 +27903,11 @@
         <v>9.7164407448105052</v>
       </c>
       <c r="DJ13" s="58">
-        <v>-22.640293427012004</v>
-      </c>
-      <c r="DK13" s="58"/>
+        <v>-22.147234779429827</v>
+      </c>
+      <c r="DK13" s="58">
+        <v>-19.219738600614811</v>
+      </c>
       <c r="DL13" s="58"/>
       <c r="DM13" s="58"/>
       <c r="DN13" s="58"/>
@@ -28265,9 +28358,11 @@
         <v>-2.5643810015893442</v>
       </c>
       <c r="DJ14" s="54">
-        <v>-1.1671698362974103</v>
-      </c>
-      <c r="DK14" s="54"/>
+        <v>-0.48639503121380434</v>
+      </c>
+      <c r="DK14" s="54">
+        <v>1.6749319092920212</v>
+      </c>
       <c r="DL14" s="54"/>
       <c r="DM14" s="54"/>
       <c r="DN14" s="54"/>
@@ -28718,9 +28813,11 @@
         <v>15.599528028887267</v>
       </c>
       <c r="DJ15" s="115">
-        <v>12.909375322064509</v>
-      </c>
-      <c r="DK15" s="115"/>
+        <v>14.73277477626327</v>
+      </c>
+      <c r="DK15" s="115">
+        <v>4.523171016015759</v>
+      </c>
       <c r="DL15" s="115"/>
       <c r="DM15" s="115"/>
       <c r="DN15" s="115"/>
@@ -28856,8 +28953,8 @@
   <dimension ref="A2:DR19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DI6" sqref="DI6:DJ15"/>
+      <pane xSplit="1" topLeftCell="DF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DJ6" sqref="DJ6:DK15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -28869,8 +28966,8 @@
     <col min="77" max="77" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="80" max="91" width="9.1796875" customWidth="1"/>
     <col min="92" max="92" width="9.81640625" customWidth="1"/>
-    <col min="93" max="114" width="9.1796875" customWidth="1"/>
-    <col min="115" max="121" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="93" max="115" width="9.1796875" customWidth="1"/>
+    <col min="116" max="121" width="9.1796875" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="28.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29522,10 +29619,10 @@
         <v>5</v>
       </c>
       <c r="DJ5" s="50" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="DK5" s="50" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="DL5" s="50" t="s">
         <v>8</v>
@@ -29998,9 +30095,11 @@
         <v>-4.2199500288139902</v>
       </c>
       <c r="DJ6" s="54">
-        <v>2.2618644421327661</v>
-      </c>
-      <c r="DK6" s="54"/>
+        <v>-3.6734749437979608</v>
+      </c>
+      <c r="DK6" s="54">
+        <v>5.0645450655960156</v>
+      </c>
       <c r="DL6" s="54"/>
       <c r="DM6" s="54"/>
       <c r="DN6" s="54"/>
@@ -30462,9 +30561,11 @@
         <v>3.3336895384901144</v>
       </c>
       <c r="DJ7" s="58">
-        <v>3.0984364466891678</v>
-      </c>
-      <c r="DK7" s="58"/>
+        <v>4.3859183121780498</v>
+      </c>
+      <c r="DK7" s="58">
+        <v>-6.4851807381510751</v>
+      </c>
       <c r="DL7" s="58"/>
       <c r="DM7" s="58"/>
       <c r="DN7" s="58"/>
@@ -30926,9 +31027,11 @@
         <v>27.401939629616745</v>
       </c>
       <c r="DJ8" s="54">
-        <v>-0.43643733493866632</v>
-      </c>
-      <c r="DK8" s="54"/>
+        <v>4.3680406542059069</v>
+      </c>
+      <c r="DK8" s="54">
+        <v>-16.789735327169787</v>
+      </c>
       <c r="DL8" s="54"/>
       <c r="DM8" s="54"/>
       <c r="DN8" s="54"/>
@@ -31390,9 +31493,11 @@
         <v>5.1510179364306907</v>
       </c>
       <c r="DJ9" s="58">
-        <v>3.7229104973903526</v>
-      </c>
-      <c r="DK9" s="58"/>
+        <v>3.6671709487393622</v>
+      </c>
+      <c r="DK9" s="58">
+        <v>-7.9288442994677411</v>
+      </c>
       <c r="DL9" s="58"/>
       <c r="DM9" s="58"/>
       <c r="DN9" s="58"/>
@@ -31854,9 +31959,11 @@
         <v>35.690529044001053</v>
       </c>
       <c r="DJ10" s="54">
-        <v>2.6827739384792659</v>
-      </c>
-      <c r="DK10" s="54"/>
+        <v>-5.5648835638744565</v>
+      </c>
+      <c r="DK10" s="54">
+        <v>-9.9897449579365869</v>
+      </c>
       <c r="DL10" s="54"/>
       <c r="DM10" s="54"/>
       <c r="DN10" s="54"/>
@@ -32318,9 +32425,11 @@
         <v>14.532878776310397</v>
       </c>
       <c r="DJ11" s="58">
-        <v>11.315114064593512</v>
-      </c>
-      <c r="DK11" s="58"/>
+        <v>7.7181478900238298</v>
+      </c>
+      <c r="DK11" s="58">
+        <v>-7.0878642429195171E-2</v>
+      </c>
       <c r="DL11" s="58"/>
       <c r="DM11" s="58"/>
       <c r="DN11" s="58"/>
@@ -32782,9 +32891,11 @@
         <v>12.770702319537609</v>
       </c>
       <c r="DJ12" s="54">
-        <v>1.7666130951409897</v>
-      </c>
-      <c r="DK12" s="54"/>
+        <v>-9.7264663555957647</v>
+      </c>
+      <c r="DK12" s="54">
+        <v>1.9254031272376126</v>
+      </c>
       <c r="DL12" s="54"/>
       <c r="DM12" s="54"/>
       <c r="DN12" s="54"/>
@@ -33246,9 +33357,11 @@
         <v>-1.7070344846823127</v>
       </c>
       <c r="DJ13" s="58">
-        <v>5.2717166409010696</v>
-      </c>
-      <c r="DK13" s="58"/>
+        <v>5.9426748507366289</v>
+      </c>
+      <c r="DK13" s="58">
+        <v>-6.6039489088649646</v>
+      </c>
       <c r="DL13" s="58"/>
       <c r="DM13" s="58"/>
       <c r="DN13" s="58"/>
@@ -33710,9 +33823,11 @@
         <v>0.83198228423280174</v>
       </c>
       <c r="DJ14" s="54">
-        <v>0.4809415176791676</v>
-      </c>
-      <c r="DK14" s="54"/>
+        <v>1.1730687517471639</v>
+      </c>
+      <c r="DK14" s="54">
+        <v>0.47353468614093064</v>
+      </c>
       <c r="DL14" s="54"/>
       <c r="DM14" s="54"/>
       <c r="DN14" s="54"/>
@@ -34174,9 +34289,11 @@
         <v>17.316482614877906</v>
       </c>
       <c r="DJ15" s="115">
-        <v>1.5833887168992034</v>
-      </c>
-      <c r="DK15" s="115"/>
+        <v>3.2238822101428921</v>
+      </c>
+      <c r="DK15" s="115">
+        <v>-11.070795556916712</v>
+      </c>
       <c r="DL15" s="115"/>
       <c r="DM15" s="115"/>
       <c r="DN15" s="115"/>
@@ -34311,10 +34428,10 @@
   <dimension ref="A2:AP20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="Z6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="AH6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AL6" sqref="AL6:AM15"/>
+      <selection pane="bottomRight" activeCell="AM6" sqref="AM6:AM15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -34574,7 +34691,7 @@
         <v>32</v>
       </c>
       <c r="AM5" s="76" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AN5" s="76" t="s">
         <v>34</v>
@@ -34707,7 +34824,7 @@
         <v>-46.928914964358512</v>
       </c>
       <c r="AM6" s="117">
-        <v>-5.2463593307737195</v>
+        <v>-13.349943140529769</v>
       </c>
       <c r="AN6" s="117"/>
       <c r="AO6" s="117"/>
@@ -34838,7 +34955,7 @@
         <v>-31.311284840063934</v>
       </c>
       <c r="AM7" s="118">
-        <v>-19.574337142448123</v>
+        <v>-19.297607058759464</v>
       </c>
       <c r="AN7" s="118"/>
       <c r="AO7" s="118"/>
@@ -34969,7 +35086,7 @@
         <v>9.0956015631321474</v>
       </c>
       <c r="AM8" s="117">
-        <v>59.704818493724368</v>
+        <v>54.680163233026867</v>
       </c>
       <c r="AN8" s="117"/>
       <c r="AO8" s="117"/>
@@ -35100,7 +35217,7 @@
         <v>-10.407784890605184</v>
       </c>
       <c r="AM9" s="118">
-        <v>13.954860304769555</v>
+        <v>12.593035064356178</v>
       </c>
       <c r="AN9" s="118"/>
       <c r="AO9" s="118"/>
@@ -35231,7 +35348,7 @@
         <v>-36.806171297280287</v>
       </c>
       <c r="AM10" s="117">
-        <v>-9.1180269742150486</v>
+        <v>-13.580927825299122</v>
       </c>
       <c r="AN10" s="117"/>
       <c r="AO10" s="117"/>
@@ -35362,7 +35479,7 @@
         <v>-3.0385913989727782</v>
       </c>
       <c r="AM11" s="118">
-        <v>50.279096657567948</v>
+        <v>46.444804151890288</v>
       </c>
       <c r="AN11" s="118"/>
       <c r="AO11" s="118"/>
@@ -35493,7 +35610,7 @@
         <v>-5.1214857728526626</v>
       </c>
       <c r="AM12" s="117">
-        <v>18.778145705957694</v>
+        <v>10.052685074908212</v>
       </c>
       <c r="AN12" s="117"/>
       <c r="AO12" s="117"/>
@@ -35624,7 +35741,7 @@
         <v>25.738496258522218</v>
       </c>
       <c r="AM13" s="118">
-        <v>-6.4619263411007495</v>
+        <v>-10.550177545078045</v>
       </c>
       <c r="AN13" s="118"/>
       <c r="AO13" s="118"/>
@@ -35755,7 +35872,7 @@
         <v>-29.230201615558354</v>
       </c>
       <c r="AM14" s="117">
-        <v>-1.8657754189433773</v>
+        <v>-0.45861470783704245</v>
       </c>
       <c r="AN14" s="117"/>
       <c r="AO14" s="117"/>
@@ -35886,7 +36003,7 @@
         <v>-16.349383050386969</v>
       </c>
       <c r="AM15" s="119">
-        <v>14.254451675475888</v>
+        <v>11.6184912737221</v>
       </c>
       <c r="AN15" s="119"/>
       <c r="AO15" s="119"/>
@@ -36025,11 +36142,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:DJ17"/>
+  <dimension ref="A2:DK17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DI13" sqref="DI13"/>
+      <pane xSplit="1" topLeftCell="DF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DK16" sqref="DK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -36039,11 +36156,11 @@
     <col min="62" max="62" width="8.81640625" collapsed="1"/>
     <col min="80" max="82" width="9.1796875" customWidth="1"/>
     <col min="83" max="83" width="9.453125" customWidth="1"/>
-    <col min="84" max="113" width="9.1796875" customWidth="1"/>
-    <col min="114" max="114" width="36.453125" customWidth="1"/>
+    <col min="84" max="114" width="9.1796875" customWidth="1"/>
+    <col min="115" max="115" width="36.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:114" s="16" customFormat="1" ht="14.5" customHeight="1">
+    <row r="2" spans="1:115" s="16" customFormat="1" ht="14.5" customHeight="1">
       <c r="A2" s="39" t="s">
         <v>72</v>
       </c>
@@ -36159,11 +36276,12 @@
       <c r="DG2" s="3"/>
       <c r="DH2" s="3"/>
       <c r="DI2" s="3"/>
-      <c r="DJ2" s="40" t="s">
+      <c r="DJ2" s="3"/>
+      <c r="DK2" s="40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:114" ht="14.5" customHeight="1" thickBot="1">
+    <row r="3" spans="1:115" ht="14.5" customHeight="1" thickBot="1">
       <c r="A3" s="14"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -36277,8 +36395,9 @@
       <c r="DG3" s="8"/>
       <c r="DH3" s="8"/>
       <c r="DI3" s="8"/>
+      <c r="DJ3" s="8"/>
     </row>
-    <row r="4" spans="1:114" ht="18" customHeight="1">
+    <row r="4" spans="1:115" ht="18" customHeight="1">
       <c r="A4" s="164" t="s">
         <v>0</v>
       </c>
@@ -36413,12 +36532,13 @@
       </c>
       <c r="DG4" s="170"/>
       <c r="DH4" s="170"/>
-      <c r="DI4" s="171"/>
-      <c r="DJ4" s="160" t="s">
+      <c r="DI4" s="170"/>
+      <c r="DJ4" s="171"/>
+      <c r="DK4" s="160" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:114" ht="18" customHeight="1">
+    <row r="5" spans="1:115" ht="18" customHeight="1">
       <c r="A5" s="165"/>
       <c r="B5" s="110" t="s">
         <v>2</v>
@@ -36756,9 +36876,12 @@
       <c r="DI5" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="DJ5" s="161"/>
+      <c r="DJ5" s="108" t="s">
+        <v>106</v>
+      </c>
+      <c r="DK5" s="161"/>
     </row>
-    <row r="6" spans="1:114" ht="18" customHeight="1" thickBot="1">
+    <row r="6" spans="1:115" ht="18" customHeight="1" thickBot="1">
       <c r="A6" s="104"/>
       <c r="B6" s="87"/>
       <c r="C6" s="88"/>
@@ -36872,9 +36995,10 @@
       <c r="DG6" s="120"/>
       <c r="DH6" s="120"/>
       <c r="DI6" s="120"/>
-      <c r="DJ6" s="90"/>
+      <c r="DJ6" s="120"/>
+      <c r="DK6" s="90"/>
     </row>
-    <row r="7" spans="1:114" ht="18" customHeight="1">
+    <row r="7" spans="1:115" ht="18" customHeight="1">
       <c r="A7" s="96" t="s">
         <v>48</v>
       </c>
@@ -36990,11 +37114,12 @@
       <c r="DG7" s="137"/>
       <c r="DH7" s="137"/>
       <c r="DI7" s="137"/>
-      <c r="DJ7" s="99" t="s">
+      <c r="DJ7" s="137"/>
+      <c r="DK7" s="99" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:114" ht="18" customHeight="1">
+    <row r="8" spans="1:115" ht="18" customHeight="1">
       <c r="A8" s="105" t="s">
         <v>49</v>
       </c>
@@ -37334,11 +37459,14 @@
       <c r="DI8" s="92">
         <v>142.44867735509126</v>
       </c>
-      <c r="DJ8" s="94" t="s">
+      <c r="DJ8" s="92">
+        <v>124.41572425792351</v>
+      </c>
+      <c r="DK8" s="94" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:114" ht="18" customHeight="1">
+    <row r="9" spans="1:115" ht="18" customHeight="1">
       <c r="A9" s="105" t="s">
         <v>50</v>
       </c>
@@ -37678,11 +37806,14 @@
       <c r="DI9" s="92">
         <v>134.00167765875364</v>
       </c>
-      <c r="DJ9" s="94" t="s">
+      <c r="DJ9" s="92">
+        <v>119.92965109127339</v>
+      </c>
+      <c r="DK9" s="94" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:114" ht="18" customHeight="1" thickBot="1">
+    <row r="10" spans="1:115" ht="18" customHeight="1" thickBot="1">
       <c r="A10" s="106"/>
       <c r="B10" s="91"/>
       <c r="C10" s="92"/>
@@ -37796,9 +37927,10 @@
       <c r="DG10" s="92"/>
       <c r="DH10" s="92"/>
       <c r="DI10" s="92"/>
-      <c r="DJ10" s="95"/>
+      <c r="DJ10" s="92"/>
+      <c r="DK10" s="95"/>
     </row>
-    <row r="11" spans="1:114" ht="18" customHeight="1">
+    <row r="11" spans="1:115" ht="18" customHeight="1">
       <c r="A11" s="96" t="s">
         <v>51</v>
       </c>
@@ -37914,11 +38046,12 @@
       <c r="DG11" s="137"/>
       <c r="DH11" s="137"/>
       <c r="DI11" s="137"/>
-      <c r="DJ11" s="99" t="s">
+      <c r="DJ11" s="137"/>
+      <c r="DK11" s="99" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:114" ht="18" customHeight="1">
+    <row r="12" spans="1:115" ht="18" customHeight="1">
       <c r="A12" s="105" t="s">
         <v>49</v>
       </c>
@@ -38258,11 +38391,14 @@
       <c r="DI12" s="92">
         <v>147.279792746114</v>
       </c>
-      <c r="DJ12" s="94" t="s">
+      <c r="DJ12" s="92">
+        <v>129.40414507772022</v>
+      </c>
+      <c r="DK12" s="94" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:114" ht="18" customHeight="1">
+    <row r="13" spans="1:115" ht="18" customHeight="1">
       <c r="A13" s="105" t="s">
         <v>50</v>
       </c>
@@ -38602,11 +38738,14 @@
       <c r="DI13" s="92">
         <v>147.92746113989637</v>
       </c>
-      <c r="DJ13" s="94" t="s">
+      <c r="DJ13" s="92">
+        <v>133.41968911917098</v>
+      </c>
+      <c r="DK13" s="94" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:114" ht="18" customHeight="1" thickBot="1">
+    <row r="14" spans="1:115" ht="18" customHeight="1" thickBot="1">
       <c r="A14" s="107"/>
       <c r="B14" s="101"/>
       <c r="C14" s="102"/>
@@ -38720,9 +38859,10 @@
       <c r="DG14" s="102"/>
       <c r="DH14" s="102"/>
       <c r="DI14" s="102"/>
-      <c r="DJ14" s="112"/>
+      <c r="DJ14" s="102"/>
+      <c r="DK14" s="112"/>
     </row>
-    <row r="15" spans="1:114" s="41" customFormat="1" ht="16.5" customHeight="1">
+    <row r="15" spans="1:115" s="41" customFormat="1" ht="16.5" customHeight="1">
       <c r="A15" s="31"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -38836,9 +38976,10 @@
       <c r="DG15" s="26"/>
       <c r="DH15" s="26"/>
       <c r="DI15" s="26"/>
-      <c r="DJ15" s="31"/>
+      <c r="DJ15" s="26"/>
+      <c r="DK15" s="31"/>
     </row>
-    <row r="16" spans="1:114" s="44" customFormat="1" ht="16.5" customHeight="1">
+    <row r="16" spans="1:115" s="44" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="31"/>
       <c r="B16" s="42"/>
       <c r="C16" s="42"/>
@@ -38951,15 +39092,16 @@
       <c r="DG16" s="29"/>
       <c r="DH16" s="29"/>
       <c r="DI16" s="29"/>
-      <c r="DJ16" s="31"/>
+      <c r="DJ16" s="29"/>
+      <c r="DK16" s="31"/>
     </row>
-    <row r="17" spans="1:114" s="44" customFormat="1" ht="14.5" customHeight="1">
+    <row r="17" spans="1:115" s="44" customFormat="1" ht="14.5" customHeight="1">
       <c r="A17" s="31"/>
-      <c r="DJ17" s="31"/>
+      <c r="DK17" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="DJ4:DJ5"/>
+    <mergeCell ref="DK4:DK5"/>
     <mergeCell ref="BJ4:BU4"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:M4"/>
@@ -38969,7 +39111,7 @@
     <mergeCell ref="AX4:BI4"/>
     <mergeCell ref="BV4:CG4"/>
     <mergeCell ref="CH4:CS4"/>
-    <mergeCell ref="DF4:DI4"/>
+    <mergeCell ref="DF4:DJ4"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>